<commit_message>
correttive a seguito di prime valutazione
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111NBSSRLXXXXX/NBS/networksanitario/v.4.10.106/report-checklist.xlsx
+++ b/GATEWAY/S1#111NBSSRLXXXXX/NBS/networksanitario/v.4.10.106/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.damiani\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.damiani\Desktop\S1#111NBSSRLXXXXX\NBS\networksanitario\v.4.10.106\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9116352-4626-4025-8A29-DFA9FF913862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859F2FFE-6F41-407B-80E3-90281C8D9E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="345" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="465" windowWidth="29040" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="123">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -492,18 +492,6 @@
     <t>il sofware non consente l' inserimento di una posizione anagrafica con un valore sesso diverso da male,femal,undefined</t>
   </si>
   <si>
-    <t>28/04/202310:47:11</t>
-  </si>
-  <si>
-    <t>28/04/202310:47:13</t>
-  </si>
-  <si>
-    <t>28/04/202310:48:13</t>
-  </si>
-  <si>
-    <t>28/04/202310:49:13</t>
-  </si>
-  <si>
     <t>il sofware non consente di effettuare la validazione del documento della lettera di dimissione ospedaliera se  non viene compilato il campo diagnosi alla dimissione</t>
   </si>
   <si>
@@ -543,9 +531,6 @@
     <t>400-Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: Z15]</t>
   </si>
   <si>
-    <t>28/04/202310:45:10</t>
-  </si>
-  <si>
     <t>28/04/2023T14:46:26Z</t>
   </si>
   <si>
@@ -562,6 +547,9 @@
   </si>
   <si>
     <t>400-Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.112 v2.1.0, Codes: Z16]</t>
+  </si>
+  <si>
+    <t>403-Il campo purpose_of_use non è valorizzato</t>
   </si>
 </sst>
 </file>
@@ -897,29 +885,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -951,6 +916,29 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1247,10 +1235,10 @@
   <dimension ref="A1:T646"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="F19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomRight" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1289,14 +1277,14 @@
       <c r="T1" s="6"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="26"/>
+      <c r="D2" s="37"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -1314,14 +1302,14 @@
       <c r="T2" s="6"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="34" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="35"/>
+      <c r="D3" s="46"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1339,12 +1327,12 @@
       <c r="T3" s="6"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="34" t="s">
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="35"/>
+      <c r="D4" s="46"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -1363,12 +1351,12 @@
       <c r="T4" s="6"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="34" t="s">
+      <c r="A5" s="43"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="35"/>
+      <c r="D5" s="46"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1386,8 +1374,8 @@
       <c r="T5" s="6"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="24"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="7"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1664,19 +1652,15 @@
       <c r="E13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="13">
-        <v>45043</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>79</v>
-      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="15" t="s">
         <v>66</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
@@ -1728,7 +1712,9 @@
       <c r="M14" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="N14" s="15"/>
+      <c r="N14" s="15" t="s">
+        <v>122</v>
+      </c>
       <c r="O14" s="15" t="s">
         <v>39</v>
       </c>
@@ -1910,12 +1896,8 @@
       <c r="E18" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="13">
-        <v>45043</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>79</v>
-      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="15" t="s">
@@ -1990,45 +1972,41 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="46" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="36">
+    <row r="20" spans="1:20" s="33" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="23">
         <v>66</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="38" t="s">
+      <c r="E20" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="39">
-        <v>45044</v>
-      </c>
-      <c r="G20" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="H20" s="41"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="42" t="s">
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="K20" s="42" t="s">
+      <c r="K20" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="43"/>
-      <c r="S20" s="44"/>
-      <c r="T20" s="45" t="s">
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="32" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2048,12 +2026,8 @@
       <c r="E21" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="13">
-        <v>45044</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>103</v>
-      </c>
+      <c r="F21" s="26"/>
+      <c r="G21" s="27"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="15" t="s">
@@ -2090,12 +2064,8 @@
       <c r="E22" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="13">
-        <v>45044</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>105</v>
-      </c>
+      <c r="F22" s="26"/>
+      <c r="G22" s="27"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="15" t="s">
@@ -2132,19 +2102,15 @@
       <c r="E23" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="13">
-        <v>45044</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>106</v>
-      </c>
+      <c r="F23" s="26"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="15" t="s">
         <v>66</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
@@ -2174,19 +2140,15 @@
       <c r="E24" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="13">
-        <v>45044</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>104</v>
-      </c>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="15" t="s">
         <v>66</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
@@ -2220,13 +2182,13 @@
         <v>45044</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J25" s="15" t="s">
         <v>39</v>
@@ -2239,7 +2201,7 @@
         <v>39</v>
       </c>
       <c r="N25" s="15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O25" s="15" t="s">
         <v>66</v>
@@ -2274,13 +2236,13 @@
         <v>45044</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="J26" s="15" t="s">
         <v>39</v>
@@ -2293,7 +2255,7 @@
         <v>39</v>
       </c>
       <c r="N26" s="15" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="O26" s="15" t="s">
         <v>66</v>
@@ -2328,13 +2290,13 @@
         <v>45044</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J27" s="15" t="s">
         <v>39</v>
@@ -2347,7 +2309,7 @@
         <v>39</v>
       </c>
       <c r="N27" s="15" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="O27" s="15" t="s">
         <v>66</v>
@@ -2382,13 +2344,13 @@
         <v>45044</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="J28" s="15" t="s">
         <v>39</v>
@@ -2401,7 +2363,7 @@
         <v>39</v>
       </c>
       <c r="N28" s="15" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="O28" s="15" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
modifiche a seguto di mancato accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111NBSSRLXXXXX/NBS/networksanitario/v.4.10.106/report-checklist.xlsx
+++ b/GATEWAY/S1#111NBSSRLXXXXX/NBS/networksanitario/v.4.10.106/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.damiani\Desktop\it-fse-accreditamento\GATEWAY\S1#111NBSSRLXXXXX\NBS\networksanitario\v.4.10.106\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.damiani\Desktop\GATEWAY\S1#111NBSSRLXXXXX\NBS\networksanitario\v.4.10.106\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE3ECEF-1DAC-465D-A938-97F1F4CBD71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB217609-4A2B-4048-AFF0-26B41C392B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="465" windowWidth="29040" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="335">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -429,88 +429,7 @@
     <t>403-Il campo purpose_of_use non è valorizzato</t>
   </si>
   <si>
-    <t>8c8f43cc9de24318</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.df1d0559856200310bac03497c5ba7f1483d77451c9bf611f9ad2a4c5328191c.217cf41ece^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>16/05/202316:24:51</t>
-  </si>
-  <si>
-    <t>b18ded85b1263f88</t>
-  </si>
-  <si>
-    <t>088b2b1c91236091</t>
-  </si>
-  <si>
-    <t>16/05/202316:29:15</t>
-  </si>
-  <si>
-    <t>400ERROREERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'languageCode'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected.</t>
-  </si>
-  <si>
-    <t>2b2cbddba6144bb1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.8145bff7ccd5b67a1a7eb1bc60ee039287b299ffa8622e1a5b0994a5d84fc3f1.348fb46450^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>16/05/202316:57:11</t>
-  </si>
-  <si>
-    <t>18/05/202311:41:06</t>
-  </si>
-  <si>
-    <t>881ac63d8298b761</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.222c9daa15cc42a5a7f858ec1474769c4d08586a8f6e3dea7e06b5b7695748f5.cc10824e73^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>7e2c490e2a41d975</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.7cfe9ca95a7a43d48ae106b386ceead8b65d08670d4e8cdd4a11ac5608322dcf.ec1bf74de7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>e633e0f281971e9b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.f056229fb4493079f283df927f79b6e6f066dfaa09ffba9a007f26cb1348aaab.edd45473ff^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b26| Sotto-sezione Anamnesi: l'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.e121c21e8a7eaa29b5d72cc45b785a32859b7e1ac715932b01fe79b23ca815eb.2f0690af08^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>f22fc4fafd2c425d</t>
-  </si>
-  <si>
-    <t>18/05/2023 15:28:19Z</t>
-  </si>
-  <si>
-    <t>0c6f8db22fd89cca</t>
-  </si>
-  <si>
-    <t>18/05/202315:49:37Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.da0d043f0024341bda9f3364781f94ed39aa7f588cffd80d41b5de35ab7f193f.36737e40f3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>c48d69dd71c32516</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.21b45100b08a16f3ff689d3f1941ab85602f6f1bc2ca8baba71fcd7d75694d71.4603109b06^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>7401e2608bcd608b</t>
-  </si>
-  <si>
-    <t>31/05/202310:25:09</t>
   </si>
   <si>
     <t>VPS</t>
@@ -560,9 +479,6 @@
     <t>VALIDAZIONE_VPS_TIMEOUT</t>
   </si>
   <si>
-    <t>00-Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.112 v2.1.0, Codes: Z16]</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_VPS_CT5_KO</t>
   </si>
   <si>
@@ -684,19 +600,7 @@
     <t>VALIDAZIONE_CDA2_VPS_CT29_KO</t>
   </si>
   <si>
-    <t>da4278baecfda4a7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.3.1.4.4.ccc97c12937e3fc73a6418f78f3e901f13350ed72befb4e5d55235a88418afaf.80bf49624b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>8342563512c878ca</t>
-  </si>
-  <si>
     <t>403-Campo token JWT non valido,Il campo purpose_of_use non è valorizzato</t>
-  </si>
-  <si>
-    <t>9fd189afccaf2260</t>
   </si>
   <si>
     <t>Attenzione!
@@ -704,15 +608,6 @@
 Tentare di nuovo il processo di validazione?</t>
   </si>
   <si>
-    <t>5dee594ca16b3830</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.3.1.4.4.4b8ebc26a9b85b640342a8b48894aa8de24b2cc27b07c6bc064ddce61bc06a12.96a810d08d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>400-ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'languageCode'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected</t>
-  </si>
-  <si>
     <t>Il software esegue controlli di congruneza del  CF e correttezza impostandolo in maiuscolo</t>
   </si>
   <si>
@@ -1136,12 +1031,6 @@
     <t>VALIDAZIONE_CDA2_RSA_CT4_OK</t>
   </si>
   <si>
-    <t>dea385d333c6fb43</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.c3431fb8c4b1c1fcd5618491edfa23049698bc24afc7a64611ee0c20f9bca273.8b75965aa1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>7d0a5395b84c49b6</t>
   </si>
   <si>
@@ -1287,16 +1176,88 @@
     <t>2.16.840.1.113883.2.9.2.110.4.4.3ef6f06ee2145e043d78951fa763bda4494f40e89021bb5220992b438cf759d2.f842d68ad3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>e2484a1fadb38678</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.3.1.4.4.ccc97c12937e3fc73a6418f78f3e901f13350ed72befb4e5d55235a88418afaf.f585945b57^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>f36e6be885d5b8bb</t>
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.110.4.4.0790ca93f8b308251521d3054e27fd1cd541f3b90688f98e34e1557513d826fe.f1a22a6220^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>10dbf1af082444ba</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.21b45100b08a16f3ff689d3f1941ab85602f6f1bc2ca8baba71fcd7d75694d71.e777996eb1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>46191492ee9ac323</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.ad22097059252407bdab5833e17c82202b26a969c562d739294be80dac4c026e.75b978f7fe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e1144768a6ee995c</t>
+  </si>
+  <si>
+    <t>61acf4a3adb47615</t>
+  </si>
+  <si>
+    <t>0fac3d264a0bb9aa</t>
+  </si>
+  <si>
+    <t>3bf0645249db3233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il software esegue controlli sul mancato inserimento del confidentialy code </t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.222c9daa15cc42a5a7f858ec1474769c4d08586a8f6e3dea7e06b5b7695748f5.2efa68cf77^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>9763a19262b32946</t>
+  </si>
+  <si>
+    <t>9d796021f8705deb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.f056229fb4493079f283df927f79b6e6f066dfaa09ffba9a007f26cb1348aaab.2d45f2023d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>9b486eee5e52ee66</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.7cfe9ca95a7a43d48ae106b386ceead8b65d08670d4e8cdd4a11ac5608322dcf.4eebe4bed9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.e121c21e8a7eaa29b5d72cc45b785a32859b7e1ac715932b01fe79b23ca815eb.e4bb7ac10c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>945ac74ccca0fd74</t>
+  </si>
+  <si>
+    <t>21/06/202312:09:35</t>
+  </si>
+  <si>
+    <t>0c4604a7218d0b31</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.da0d043f0024341bda9f3364781f94ed39aa7f588cffd80d41b5de35ab7f193f.f0befbe2cf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>400-Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.112 v2.1.0, Codes: Z16]</t>
+  </si>
+  <si>
+    <t>760b4aad219d153f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.3ef6f06ee2145e043d78951fa763bda4494f40e89021bb5220992b438cf759d2.6ae9b446b0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>a499eba6c659a277</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.0790ca93f8b308251521d3054e27fd1cd541f3b90688f98e34e1557513d826fe.022ca9bbe1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -2026,10 +1987,10 @@
   <dimension ref="A1:U709"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B85" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I86" sqref="I86"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2306,10 +2267,10 @@
         <v>45093.414282407408</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>342</v>
+        <v>305</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>343</v>
+        <v>306</v>
       </c>
       <c r="J10" s="15" t="s">
         <v>38</v>
@@ -2348,16 +2309,16 @@
         <v>29</v>
       </c>
       <c r="F11" s="13">
-        <v>45076</v>
+        <v>45097</v>
       </c>
       <c r="G11" s="14">
-        <v>45076.753506944442</v>
+        <v>45097.962847222225</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>110</v>
+        <v>309</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>111</v>
+        <v>310</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>38</v>
@@ -2396,16 +2357,16 @@
         <v>31</v>
       </c>
       <c r="F12" s="13">
-        <v>45077</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>113</v>
+        <v>45097</v>
+      </c>
+      <c r="G12" s="14">
+        <v>45097.967002314814</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>112</v>
+        <v>311</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>111</v>
+        <v>312</v>
       </c>
       <c r="J12" s="20" t="s">
         <v>38</v>
@@ -2455,7 +2416,9 @@
       </c>
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
+      <c r="N13" s="15" t="s">
+        <v>334</v>
+      </c>
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
@@ -2473,39 +2436,29 @@
         <v>25</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="F14" s="13">
-        <v>45093</v>
-      </c>
-      <c r="G14" s="14">
-        <v>45093.41946759259</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>345</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
       <c r="J14" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="K14" s="15"/>
+        <v>65</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>84</v>
+      </c>
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
       <c r="N14" s="15"/>
-      <c r="O14" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="P14" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
       <c r="R14" s="16"/>
       <c r="S14" s="17"/>
@@ -2521,13 +2474,13 @@
         <v>25</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="14"/>
@@ -2537,7 +2490,7 @@
         <v>65</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
@@ -2559,13 +2512,13 @@
         <v>25</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="14"/>
@@ -2575,7 +2528,7 @@
         <v>65</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
@@ -2597,13 +2550,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="14"/>
@@ -2613,7 +2566,7 @@
         <v>65</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
@@ -2644,13 +2597,13 @@
         <v>35</v>
       </c>
       <c r="F18" s="13">
-        <v>45062</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>88</v>
+        <v>45098</v>
+      </c>
+      <c r="G18" s="14">
+        <v>45098.452708333331</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>89</v>
+        <v>313</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>66</v>
@@ -2689,13 +2642,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="F19" s="13">
         <v>45090</v>
@@ -2704,7 +2657,7 @@
         <v>45090.697604166664</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>238</v>
+        <v>203</v>
       </c>
       <c r="I19" s="14" t="s">
         <v>66</v>
@@ -2743,22 +2696,22 @@
         <v>25</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="F20" s="13">
-        <v>45082</v>
+        <v>45098</v>
       </c>
       <c r="G20" s="14">
-        <v>45082.732939814814</v>
+        <v>45098.455891203703</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>166</v>
+        <v>314</v>
       </c>
       <c r="I20" s="14" t="s">
         <v>66</v>
@@ -2774,7 +2727,7 @@
         <v>38</v>
       </c>
       <c r="N20" s="15" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
       <c r="O20" s="15" t="s">
         <v>38</v>
@@ -2806,13 +2759,13 @@
         <v>37</v>
       </c>
       <c r="F21" s="13">
-        <v>45062</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>91</v>
+        <v>45098</v>
+      </c>
+      <c r="G21" s="14">
+        <v>45098.461597222224</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>90</v>
+        <v>316</v>
       </c>
       <c r="I21" s="14" t="s">
         <v>66</v>
@@ -2853,13 +2806,13 @@
         <v>25</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="F22" s="13">
         <v>45090</v>
@@ -2868,7 +2821,7 @@
         <v>45090.707407407404</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
       <c r="I22" s="14" t="s">
         <v>66</v>
@@ -2884,7 +2837,7 @@
         <v>38</v>
       </c>
       <c r="N22" s="15" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="O22" s="15" t="s">
         <v>38</v>
@@ -2907,22 +2860,22 @@
         <v>25</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="F23" s="13">
-        <v>45082</v>
+        <v>45098</v>
       </c>
       <c r="G23" s="14">
-        <v>45082.739374999997</v>
+        <v>45098.459108796298</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>168</v>
+        <v>315</v>
       </c>
       <c r="I23" s="14" t="s">
         <v>66</v>
@@ -2969,13 +2922,13 @@
         <v>39</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="F24" s="13">
         <v>45062</v>
       </c>
-      <c r="G24" s="14" t="s">
-        <v>91</v>
+      <c r="G24" s="14">
+        <v>45062.686979166669</v>
       </c>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
@@ -2990,7 +2943,7 @@
         <v>38</v>
       </c>
       <c r="N24" s="15" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="O24" s="15" t="s">
         <v>38</v>
@@ -3013,13 +2966,13 @@
         <v>25</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="F25" s="13">
         <v>45090</v>
@@ -3040,7 +2993,7 @@
         <v>38</v>
       </c>
       <c r="N25" s="15" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="O25" s="15" t="s">
         <v>38</v>
@@ -3063,13 +3016,13 @@
         <v>25</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>241</v>
+        <v>206</v>
       </c>
       <c r="F26" s="13">
         <v>45082</v>
@@ -3090,7 +3043,7 @@
         <v>38</v>
       </c>
       <c r="N26" s="15" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="O26" s="15" t="s">
         <v>38</v>
@@ -3120,37 +3073,21 @@
       <c r="E27" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="13">
-        <v>45062</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>94</v>
-      </c>
+      <c r="F27" s="13"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
       <c r="J27" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="M27" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="N27" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="O27" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="P27" s="15" t="s">
-        <v>74</v>
-      </c>
+      <c r="K27" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
       <c r="R27" s="16"/>
       <c r="S27" s="17"/>
@@ -3182,7 +3119,7 @@
         <v>65</v>
       </c>
       <c r="K28" s="15" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
@@ -3213,16 +3150,16 @@
         <v>44</v>
       </c>
       <c r="F29" s="13">
-        <v>45064</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>96</v>
+        <v>45098</v>
+      </c>
+      <c r="G29" s="14">
+        <v>45098.499155092592</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>97</v>
+        <v>319</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>98</v>
+        <v>318</v>
       </c>
       <c r="J29" s="15" t="s">
         <v>38</v>
@@ -3457,16 +3394,16 @@
         <v>56</v>
       </c>
       <c r="F35" s="13">
-        <v>45064</v>
+        <v>45098</v>
       </c>
       <c r="G35" s="14">
-        <v>45064.626828703702</v>
+        <v>45098.500625000001</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>101</v>
+        <v>320</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>102</v>
+        <v>321</v>
       </c>
       <c r="J35" s="36" t="s">
         <v>38</v>
@@ -3479,7 +3416,7 @@
         <v>38</v>
       </c>
       <c r="N35" s="15" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="O35" s="15" t="s">
         <v>65</v>
@@ -3511,16 +3448,16 @@
         <v>58</v>
       </c>
       <c r="F36" s="13">
-        <v>45064</v>
+        <v>45098</v>
       </c>
       <c r="G36" s="14">
-        <v>45064.608437499999</v>
+        <v>45098.502395833333</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>99</v>
+        <v>322</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>100</v>
+        <v>323</v>
       </c>
       <c r="J36" s="15" t="s">
         <v>38</v>
@@ -3565,16 +3502,16 @@
         <v>60</v>
       </c>
       <c r="F37" s="13">
-        <v>45064</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>106</v>
+        <v>45098</v>
+      </c>
+      <c r="G37" s="14">
+        <v>45067.504247685189</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>105</v>
+        <v>325</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>104</v>
+        <v>324</v>
       </c>
       <c r="J37" s="15" t="s">
         <v>38</v>
@@ -3619,16 +3556,16 @@
         <v>62</v>
       </c>
       <c r="F38" s="13">
-        <v>45064</v>
+        <v>45098</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>108</v>
+        <v>326</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>107</v>
+        <v>327</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>109</v>
+        <v>328</v>
       </c>
       <c r="J38" s="15" t="s">
         <v>38</v>
@@ -3641,7 +3578,7 @@
         <v>38</v>
       </c>
       <c r="N38" s="15" t="s">
-        <v>127</v>
+        <v>329</v>
       </c>
       <c r="O38" s="15" t="s">
         <v>65</v>
@@ -3664,45 +3601,29 @@
         <v>25</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="F39" s="13">
-        <v>45082</v>
-      </c>
-      <c r="G39" s="14">
-        <v>45082.759108796294</v>
-      </c>
-      <c r="H39" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="I39" s="14" t="s">
-        <v>171</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="F39" s="13"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
       <c r="J39" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="M39" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="N39" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="O39" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="P39" s="15" t="s">
-        <v>74</v>
-      </c>
+      <c r="K39" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
       <c r="Q39" s="15"/>
       <c r="R39" s="16"/>
       <c r="S39" s="17"/>
@@ -3718,13 +3639,13 @@
         <v>25</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="F40" s="13"/>
       <c r="G40" s="14"/>
@@ -3734,7 +3655,7 @@
         <v>65</v>
       </c>
       <c r="K40" s="15" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
@@ -3756,13 +3677,13 @@
         <v>25</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="F41" s="13">
         <v>45082</v>
@@ -3771,10 +3692,10 @@
         <v>45082.780578703707</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="J41" s="15" t="s">
         <v>38</v>
@@ -3809,13 +3730,13 @@
         <v>25</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="F42" s="13"/>
       <c r="G42" s="14"/>
@@ -3825,7 +3746,7 @@
         <v>65</v>
       </c>
       <c r="K42" s="15" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
@@ -3847,13 +3768,13 @@
         <v>25</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="F43" s="13"/>
       <c r="G43" s="14"/>
@@ -3863,7 +3784,7 @@
         <v>65</v>
       </c>
       <c r="K43" s="15" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
@@ -3885,13 +3806,13 @@
         <v>25</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="F44" s="13"/>
       <c r="G44" s="14"/>
@@ -3923,13 +3844,13 @@
         <v>25</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="F45" s="13"/>
       <c r="G45" s="14"/>
@@ -3939,7 +3860,7 @@
         <v>65</v>
       </c>
       <c r="K45" s="15" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="L45" s="15"/>
       <c r="M45" s="15"/>
@@ -3961,13 +3882,13 @@
         <v>25</v>
       </c>
       <c r="C46" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" s="12" t="s">
         <v>114</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>142</v>
       </c>
       <c r="F46" s="13">
         <v>45083</v>
@@ -3976,10 +3897,10 @@
         <v>45083.621504629627</v>
       </c>
       <c r="H46" s="37" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="J46" s="15" t="s">
         <v>38</v>
@@ -3992,7 +3913,7 @@
         <v>38</v>
       </c>
       <c r="N46" s="15" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="O46" s="15" t="s">
         <v>65</v>
@@ -4015,13 +3936,13 @@
         <v>25</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="F47" s="13">
         <v>45083</v>
@@ -4030,10 +3951,10 @@
         <v>45083.63318287037</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="J47" s="15" t="s">
         <v>38</v>
@@ -4046,7 +3967,7 @@
         <v>38</v>
       </c>
       <c r="N47" s="15" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="O47" s="15" t="s">
         <v>65</v>
@@ -4069,13 +3990,13 @@
         <v>25</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="F48" s="13">
         <v>45083</v>
@@ -4084,10 +4005,10 @@
         <v>45083.690127314818</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="J48" s="15" t="s">
         <v>38</v>
@@ -4100,7 +4021,7 @@
         <v>38</v>
       </c>
       <c r="N48" s="15" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
       <c r="O48" s="15" t="s">
         <v>65</v>
@@ -4123,13 +4044,13 @@
         <v>25</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="F49" s="13">
         <v>45083</v>
@@ -4138,10 +4059,10 @@
         <v>45083.710844907408</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
       <c r="J49" s="15" t="s">
         <v>38</v>
@@ -4154,7 +4075,7 @@
         <v>38</v>
       </c>
       <c r="N49" s="15" t="s">
-        <v>190</v>
+        <v>155</v>
       </c>
       <c r="O49" s="15" t="s">
         <v>65</v>
@@ -4177,13 +4098,13 @@
         <v>25</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="14"/>
@@ -4193,7 +4114,7 @@
         <v>65</v>
       </c>
       <c r="K50" s="15" t="s">
-        <v>204</v>
+        <v>169</v>
       </c>
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
@@ -4215,13 +4136,13 @@
         <v>25</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="F51" s="13"/>
       <c r="G51" s="14"/>
@@ -4231,7 +4152,7 @@
         <v>65</v>
       </c>
       <c r="K51" s="15" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
@@ -4253,13 +4174,13 @@
         <v>25</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
       <c r="F52" s="13">
         <v>45084</v>
@@ -4268,10 +4189,10 @@
         <v>45084.426354166666</v>
       </c>
       <c r="H52" s="14" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>207</v>
+        <v>172</v>
       </c>
       <c r="J52" s="15" t="s">
         <v>38</v>
@@ -4284,7 +4205,7 @@
         <v>38</v>
       </c>
       <c r="N52" s="15" t="s">
-        <v>208</v>
+        <v>173</v>
       </c>
       <c r="O52" s="15" t="s">
         <v>65</v>
@@ -4307,13 +4228,13 @@
         <v>25</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="F53" s="13"/>
       <c r="G53" s="14"/>
@@ -4323,7 +4244,7 @@
         <v>65</v>
       </c>
       <c r="K53" s="15" t="s">
-        <v>209</v>
+        <v>174</v>
       </c>
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
@@ -4344,13 +4265,13 @@
         <v>25</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
       <c r="F54" s="13">
         <v>45084</v>
@@ -4359,10 +4280,10 @@
         <v>45084.446574074071</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>210</v>
+        <v>175</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
       <c r="J54" s="15" t="s">
         <v>38</v>
@@ -4375,7 +4296,7 @@
         <v>38</v>
       </c>
       <c r="N54" s="15" t="s">
-        <v>212</v>
+        <v>177</v>
       </c>
       <c r="O54" s="15" t="s">
         <v>65</v>
@@ -4398,25 +4319,25 @@
         <v>25</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>196</v>
+        <v>161</v>
       </c>
       <c r="F55" s="13">
         <v>45084</v>
       </c>
       <c r="G55" s="14" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>214</v>
+        <v>179</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>215</v>
+        <v>180</v>
       </c>
       <c r="J55" s="15" t="s">
         <v>38</v>
@@ -4429,7 +4350,7 @@
         <v>38</v>
       </c>
       <c r="N55" s="15" t="s">
-        <v>216</v>
+        <v>181</v>
       </c>
       <c r="O55" s="15" t="s">
         <v>65</v>
@@ -4452,13 +4373,13 @@
         <v>25</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>197</v>
+        <v>162</v>
       </c>
       <c r="F56" s="13"/>
       <c r="G56" s="14"/>
@@ -4468,7 +4389,7 @@
         <v>65</v>
       </c>
       <c r="K56" s="15" t="s">
-        <v>217</v>
+        <v>182</v>
       </c>
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
@@ -4490,13 +4411,13 @@
         <v>25</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="F57" s="13"/>
       <c r="G57" s="14"/>
@@ -4506,7 +4427,7 @@
         <v>65</v>
       </c>
       <c r="K57" s="15" t="s">
-        <v>218</v>
+        <v>183</v>
       </c>
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
@@ -4528,13 +4449,13 @@
         <v>25</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>199</v>
+        <v>164</v>
       </c>
       <c r="F58" s="13">
         <v>45084</v>
@@ -4543,10 +4464,10 @@
         <v>45084.511331018519</v>
       </c>
       <c r="H58" s="14" t="s">
-        <v>219</v>
+        <v>184</v>
       </c>
       <c r="I58" s="38" t="s">
-        <v>220</v>
+        <v>185</v>
       </c>
       <c r="J58" s="15" t="s">
         <v>38</v>
@@ -4559,7 +4480,7 @@
         <v>38</v>
       </c>
       <c r="N58" s="15" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="O58" s="15" t="s">
         <v>65</v>
@@ -4582,13 +4503,13 @@
         <v>25</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="F59" s="13">
         <v>45084</v>
@@ -4597,10 +4518,10 @@
         <v>45084.618067129632</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="I59" s="14" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="J59" s="15" t="s">
         <v>38</v>
@@ -4613,7 +4534,7 @@
         <v>38</v>
       </c>
       <c r="N59" s="15" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="O59" s="15" t="s">
         <v>65</v>
@@ -4636,13 +4557,13 @@
         <v>25</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>201</v>
+        <v>166</v>
       </c>
       <c r="F60" s="13">
         <v>45084</v>
@@ -4651,10 +4572,10 @@
         <v>45084.637361111112</v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>225</v>
+        <v>190</v>
       </c>
       <c r="I60" s="14" t="s">
-        <v>226</v>
+        <v>191</v>
       </c>
       <c r="J60" s="15" t="s">
         <v>38</v>
@@ -4667,7 +4588,7 @@
         <v>38</v>
       </c>
       <c r="N60" s="15" t="s">
-        <v>227</v>
+        <v>192</v>
       </c>
       <c r="O60" s="15" t="s">
         <v>65</v>
@@ -4690,13 +4611,13 @@
         <v>25</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="F61" s="13">
         <v>45084</v>
@@ -4705,10 +4626,10 @@
         <v>45084.650671296295</v>
       </c>
       <c r="H61" s="14" t="s">
-        <v>228</v>
+        <v>193</v>
       </c>
       <c r="I61" s="14" t="s">
-        <v>229</v>
+        <v>194</v>
       </c>
       <c r="J61" s="15" t="s">
         <v>38</v>
@@ -4721,7 +4642,7 @@
         <v>38</v>
       </c>
       <c r="N61" s="15" t="s">
-        <v>230</v>
+        <v>195</v>
       </c>
       <c r="O61" s="15" t="s">
         <v>65</v>
@@ -4744,13 +4665,13 @@
         <v>25</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>203</v>
+        <v>168</v>
       </c>
       <c r="F62" s="13"/>
       <c r="G62" s="14"/>
@@ -4760,7 +4681,7 @@
         <v>65</v>
       </c>
       <c r="K62" s="15" t="s">
-        <v>217</v>
+        <v>182</v>
       </c>
       <c r="L62" s="15"/>
       <c r="M62" s="15"/>
@@ -4782,13 +4703,13 @@
         <v>25</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="F63" s="13">
         <v>45084</v>
@@ -4797,10 +4718,10 @@
         <v>45084.668726851851</v>
       </c>
       <c r="H63" s="14" t="s">
-        <v>231</v>
+        <v>196</v>
       </c>
       <c r="I63" s="14" t="s">
-        <v>232</v>
+        <v>197</v>
       </c>
       <c r="J63" s="15" t="s">
         <v>38</v>
@@ -4813,7 +4734,7 @@
         <v>38</v>
       </c>
       <c r="N63" s="15" t="s">
-        <v>233</v>
+        <v>198</v>
       </c>
       <c r="O63" s="15" t="s">
         <v>65</v>
@@ -4836,13 +4757,13 @@
         <v>25</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="F64" s="13">
         <v>45093</v>
@@ -4851,10 +4772,10 @@
         <v>45093.44085648148</v>
       </c>
       <c r="H64" s="14" t="s">
-        <v>346</v>
+        <v>307</v>
       </c>
       <c r="I64" s="14" t="s">
-        <v>347</v>
+        <v>308</v>
       </c>
       <c r="J64" s="15" t="s">
         <v>38</v>
@@ -4884,39 +4805,29 @@
         <v>25</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>254</v>
+        <v>219</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="F65" s="13">
-        <v>45092</v>
-      </c>
-      <c r="G65" s="14">
-        <v>45092.440694444442</v>
-      </c>
-      <c r="H65" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="I65" s="14" t="s">
-        <v>295</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="F65" s="13"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
       <c r="J65" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="K65" s="15"/>
+        <v>65</v>
+      </c>
+      <c r="K65" s="15" t="s">
+        <v>199</v>
+      </c>
       <c r="L65" s="15"/>
       <c r="M65" s="15"/>
       <c r="N65" s="15"/>
-      <c r="O65" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="P65" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="O65" s="15"/>
+      <c r="P65" s="15"/>
       <c r="Q65" s="15"/>
       <c r="R65" s="16"/>
       <c r="S65" s="17"/>
@@ -4932,13 +4843,13 @@
         <v>25</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
       <c r="F66" s="13"/>
       <c r="G66" s="14"/>
@@ -4948,7 +4859,7 @@
         <v>65</v>
       </c>
       <c r="K66" s="15" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="L66" s="15"/>
       <c r="M66" s="15"/>
@@ -4970,13 +4881,13 @@
         <v>25</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
       <c r="F67" s="13"/>
       <c r="G67" s="14"/>
@@ -4986,7 +4897,7 @@
         <v>65</v>
       </c>
       <c r="K67" s="15" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="L67" s="15"/>
       <c r="M67" s="15"/>
@@ -5008,13 +4919,13 @@
         <v>25</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>276</v>
+        <v>241</v>
       </c>
       <c r="F68" s="13">
         <v>45092</v>
@@ -5023,10 +4934,10 @@
         <v>45092.45752314815</v>
       </c>
       <c r="H68" s="14" t="s">
-        <v>296</v>
+        <v>259</v>
       </c>
       <c r="I68" s="14" t="s">
-        <v>297</v>
+        <v>260</v>
       </c>
       <c r="J68" s="15" t="s">
         <v>38</v>
@@ -5039,7 +4950,7 @@
         <v>38</v>
       </c>
       <c r="N68" s="15" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="O68" s="15" t="s">
         <v>65</v>
@@ -5062,13 +4973,13 @@
         <v>25</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>258</v>
+        <v>223</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>277</v>
+        <v>242</v>
       </c>
       <c r="F69" s="13"/>
       <c r="G69" s="14"/>
@@ -5078,7 +4989,7 @@
         <v>65</v>
       </c>
       <c r="K69" s="15" t="s">
-        <v>299</v>
+        <v>262</v>
       </c>
       <c r="L69" s="15"/>
       <c r="M69" s="15"/>
@@ -5100,13 +5011,13 @@
         <v>25</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="F70" s="13">
         <v>45092</v>
@@ -5115,10 +5026,10 @@
         <v>45092.485243055555</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>300</v>
+        <v>263</v>
       </c>
       <c r="I70" s="14" t="s">
-        <v>301</v>
+        <v>264</v>
       </c>
       <c r="J70" s="15" t="s">
         <v>38</v>
@@ -5131,7 +5042,7 @@
         <v>38</v>
       </c>
       <c r="N70" s="15" t="s">
-        <v>302</v>
+        <v>265</v>
       </c>
       <c r="O70" s="15" t="s">
         <v>65</v>
@@ -5154,13 +5065,13 @@
         <v>25</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="F71" s="13"/>
       <c r="G71" s="14"/>
@@ -5170,7 +5081,7 @@
         <v>65</v>
       </c>
       <c r="K71" s="15" t="s">
-        <v>303</v>
+        <v>266</v>
       </c>
       <c r="L71" s="15"/>
       <c r="M71" s="15"/>
@@ -5192,13 +5103,13 @@
         <v>25</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>279</v>
+        <v>244</v>
       </c>
       <c r="F72" s="13"/>
       <c r="G72" s="14"/>
@@ -5208,7 +5119,7 @@
         <v>65</v>
       </c>
       <c r="K72" s="15" t="s">
-        <v>304</v>
+        <v>267</v>
       </c>
       <c r="L72" s="15"/>
       <c r="M72" s="15"/>
@@ -5230,13 +5141,13 @@
         <v>25</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>262</v>
+        <v>227</v>
       </c>
       <c r="E73" s="12" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
       <c r="F73" s="13"/>
       <c r="G73" s="14"/>
@@ -5246,7 +5157,7 @@
         <v>65</v>
       </c>
       <c r="K73" s="15" t="s">
-        <v>305</v>
+        <v>268</v>
       </c>
       <c r="L73" s="15"/>
       <c r="M73" s="15"/>
@@ -5268,13 +5179,13 @@
         <v>25</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
       <c r="F74" s="13"/>
       <c r="G74" s="14"/>
@@ -5284,7 +5195,7 @@
         <v>65</v>
       </c>
       <c r="K74" s="15" t="s">
-        <v>306</v>
+        <v>269</v>
       </c>
       <c r="L74" s="15"/>
       <c r="M74" s="15"/>
@@ -5306,13 +5217,13 @@
         <v>25</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="F75" s="13">
         <v>45092</v>
@@ -5321,10 +5232,10 @@
         <v>45092.527453703704</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>307</v>
+        <v>270</v>
       </c>
       <c r="I75" s="14" t="s">
-        <v>308</v>
+        <v>271</v>
       </c>
       <c r="J75" s="15" t="s">
         <v>38</v>
@@ -5337,7 +5248,7 @@
         <v>38</v>
       </c>
       <c r="N75" s="15" t="s">
-        <v>309</v>
+        <v>272</v>
       </c>
       <c r="O75" s="15" t="s">
         <v>65</v>
@@ -5360,13 +5271,13 @@
         <v>25</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>265</v>
+        <v>230</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="F76" s="13">
         <v>45092</v>
@@ -5375,10 +5286,10 @@
         <v>45092.536736111113</v>
       </c>
       <c r="H76" s="14" t="s">
-        <v>310</v>
+        <v>273</v>
       </c>
       <c r="I76" s="14" t="s">
-        <v>311</v>
+        <v>274</v>
       </c>
       <c r="J76" s="15" t="s">
         <v>38</v>
@@ -5391,7 +5302,7 @@
         <v>38</v>
       </c>
       <c r="N76" s="15" t="s">
-        <v>312</v>
+        <v>275</v>
       </c>
       <c r="O76" s="15" t="s">
         <v>65</v>
@@ -5414,13 +5325,13 @@
         <v>25</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="F77" s="13">
         <v>45092</v>
@@ -5429,10 +5340,10 @@
         <v>45092.622465277775</v>
       </c>
       <c r="H77" s="14" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
       <c r="I77" s="14" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
       <c r="J77" s="15" t="s">
         <v>38</v>
@@ -5445,7 +5356,7 @@
         <v>38</v>
       </c>
       <c r="N77" s="15" t="s">
-        <v>313</v>
+        <v>276</v>
       </c>
       <c r="O77" s="15" t="s">
         <v>65</v>
@@ -5468,13 +5379,13 @@
         <v>25</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="F78" s="13">
         <v>45092</v>
@@ -5483,10 +5394,10 @@
         <v>45092.643865740742</v>
       </c>
       <c r="H78" s="14" t="s">
-        <v>316</v>
+        <v>279</v>
       </c>
       <c r="I78" s="14" t="s">
-        <v>317</v>
+        <v>280</v>
       </c>
       <c r="J78" s="15" t="s">
         <v>38</v>
@@ -5499,7 +5410,7 @@
         <v>38</v>
       </c>
       <c r="N78" s="15" t="s">
-        <v>318</v>
+        <v>281</v>
       </c>
       <c r="O78" s="15" t="s">
         <v>65</v>
@@ -5522,13 +5433,13 @@
         <v>25</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>268</v>
+        <v>233</v>
       </c>
       <c r="E79" s="12" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="F79" s="13">
         <v>45092</v>
@@ -5537,10 +5448,10 @@
         <v>45092.6562037037</v>
       </c>
       <c r="H79" s="14" t="s">
-        <v>319</v>
+        <v>282</v>
       </c>
       <c r="I79" s="14" t="s">
-        <v>320</v>
+        <v>283</v>
       </c>
       <c r="J79" s="15" t="s">
         <v>38</v>
@@ -5553,7 +5464,7 @@
         <v>38</v>
       </c>
       <c r="N79" s="15" t="s">
-        <v>321</v>
+        <v>284</v>
       </c>
       <c r="O79" s="15" t="s">
         <v>65</v>
@@ -5576,13 +5487,13 @@
         <v>25</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>269</v>
+        <v>234</v>
       </c>
       <c r="E80" s="12" t="s">
-        <v>287</v>
+        <v>252</v>
       </c>
       <c r="F80" s="13"/>
       <c r="G80" s="14"/>
@@ -5592,7 +5503,7 @@
         <v>65</v>
       </c>
       <c r="K80" s="15" t="s">
-        <v>322</v>
+        <v>285</v>
       </c>
       <c r="L80" s="15"/>
       <c r="M80" s="15"/>
@@ -5614,13 +5525,13 @@
         <v>25</v>
       </c>
       <c r="C81" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="D81" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="D81" s="11" t="s">
-        <v>270</v>
-      </c>
       <c r="E81" s="12" t="s">
-        <v>288</v>
+        <v>253</v>
       </c>
       <c r="F81" s="13">
         <v>45092</v>
@@ -5629,10 +5540,10 @@
         <v>45092.669351851851</v>
       </c>
       <c r="H81" s="14" t="s">
-        <v>323</v>
+        <v>286</v>
       </c>
       <c r="I81" s="14" t="s">
-        <v>324</v>
+        <v>287</v>
       </c>
       <c r="J81" s="15" t="s">
         <v>38</v>
@@ -5645,7 +5556,7 @@
         <v>38</v>
       </c>
       <c r="N81" s="15" t="s">
-        <v>325</v>
+        <v>288</v>
       </c>
       <c r="O81" s="15" t="s">
         <v>65</v>
@@ -5668,13 +5579,13 @@
         <v>25</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>271</v>
+        <v>236</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
       <c r="F82" s="13">
         <v>45092</v>
@@ -5683,10 +5594,10 @@
         <v>45092.677546296298</v>
       </c>
       <c r="H82" s="14" t="s">
-        <v>326</v>
+        <v>289</v>
       </c>
       <c r="I82" s="14" t="s">
-        <v>327</v>
+        <v>290</v>
       </c>
       <c r="J82" s="15" t="s">
         <v>38</v>
@@ -5699,7 +5610,7 @@
         <v>38</v>
       </c>
       <c r="N82" s="15" t="s">
-        <v>328</v>
+        <v>291</v>
       </c>
       <c r="O82" s="15" t="s">
         <v>65</v>
@@ -5722,13 +5633,13 @@
         <v>25</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>272</v>
+        <v>237</v>
       </c>
       <c r="E83" s="12" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="F83" s="13">
         <v>45092</v>
@@ -5737,10 +5648,10 @@
         <v>45092.683692129627</v>
       </c>
       <c r="H83" s="14" t="s">
-        <v>329</v>
+        <v>292</v>
       </c>
       <c r="I83" s="14" t="s">
-        <v>330</v>
+        <v>293</v>
       </c>
       <c r="J83" s="15" t="s">
         <v>38</v>
@@ -5753,7 +5664,7 @@
         <v>38</v>
       </c>
       <c r="N83" s="15" t="s">
-        <v>331</v>
+        <v>294</v>
       </c>
       <c r="O83" s="15" t="s">
         <v>65</v>
@@ -5776,13 +5687,13 @@
         <v>25</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="F84" s="13">
         <v>45092</v>
@@ -5791,10 +5702,10 @@
         <v>45092.694479166668</v>
       </c>
       <c r="H84" s="14" t="s">
-        <v>332</v>
+        <v>295</v>
       </c>
       <c r="I84" s="14" t="s">
-        <v>333</v>
+        <v>296</v>
       </c>
       <c r="J84" s="15" t="s">
         <v>38</v>
@@ -5807,7 +5718,7 @@
         <v>38</v>
       </c>
       <c r="N84" s="15" t="s">
-        <v>334</v>
+        <v>297</v>
       </c>
       <c r="O84" s="15" t="s">
         <v>65</v>
@@ -5830,13 +5741,13 @@
         <v>25</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>274</v>
+        <v>239</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>292</v>
+        <v>257</v>
       </c>
       <c r="F85" s="13"/>
       <c r="G85" s="14"/>
@@ -5846,7 +5757,7 @@
         <v>65</v>
       </c>
       <c r="K85" s="15" t="s">
-        <v>322</v>
+        <v>285</v>
       </c>
       <c r="L85" s="15"/>
       <c r="M85" s="15"/>
@@ -5868,13 +5779,13 @@
         <v>25</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>275</v>
+        <v>240</v>
       </c>
       <c r="E86" s="12" t="s">
-        <v>338</v>
+        <v>301</v>
       </c>
       <c r="F86" s="13">
         <v>45092</v>
@@ -5883,10 +5794,10 @@
         <v>45092.703912037039</v>
       </c>
       <c r="H86" s="14" t="s">
-        <v>335</v>
+        <v>298</v>
       </c>
       <c r="I86" s="14" t="s">
-        <v>336</v>
+        <v>299</v>
       </c>
       <c r="J86" s="15" t="s">
         <v>38</v>
@@ -5899,7 +5810,7 @@
         <v>38</v>
       </c>
       <c r="N86" s="15" t="s">
-        <v>337</v>
+        <v>300</v>
       </c>
       <c r="O86" s="15" t="s">
         <v>65</v>
@@ -5925,20 +5836,20 @@
         <v>24</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>339</v>
+        <v>302</v>
       </c>
       <c r="E87" s="12"/>
       <c r="F87" s="13">
-        <v>45058</v>
+        <v>45098</v>
       </c>
       <c r="G87" s="14">
-        <v>45058.617442129631</v>
+        <v>45098.52034722222</v>
       </c>
       <c r="H87" s="14" t="s">
-        <v>86</v>
+        <v>330</v>
       </c>
       <c r="I87" s="14" t="s">
-        <v>87</v>
+        <v>331</v>
       </c>
       <c r="J87" s="15" t="s">
         <v>38</v>
@@ -5968,23 +5879,23 @@
         <v>25</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>340</v>
+        <v>303</v>
       </c>
       <c r="E88" s="12"/>
       <c r="F88" s="13">
-        <v>45082</v>
+        <v>45098</v>
       </c>
       <c r="G88" s="14">
-        <v>45082.606840277775</v>
+        <v>45098.524108796293</v>
       </c>
       <c r="H88" s="14" t="s">
-        <v>164</v>
+        <v>332</v>
       </c>
       <c r="I88" s="14" t="s">
-        <v>165</v>
+        <v>333</v>
       </c>
       <c r="J88" s="15" t="s">
         <v>38</v>
@@ -6014,23 +5925,23 @@
         <v>25</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>341</v>
+        <v>304</v>
       </c>
       <c r="E89" s="12"/>
       <c r="F89" s="13">
         <v>45090</v>
       </c>
       <c r="G89" s="14">
-        <v>45090.679467592592</v>
+        <v>45090.523912037039</v>
       </c>
       <c r="H89" s="14" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
       <c r="I89" s="14" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
       <c r="J89" s="15" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
modifiche a segito di  segnalazione
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111NBSSRLXXXXX/NBS/networksanitario/v.4.10.106/report-checklist.xlsx
+++ b/GATEWAY/S1#111NBSSRLXXXXX/NBS/networksanitario/v.4.10.106/report-checklist.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.damiani\Desktop\GATEWAY\S1#111NBSSRLXXXXX\NBS\networksanitario\v.4.10.106\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.damiani\Desktop\it-fse-accreditamento\GATEWAY\S1#111NBSSRLXXXXX\NBS\networksanitario\v.4.10.106\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB217609-4A2B-4048-AFF0-26B41C392B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0826C7F-57F2-4CD5-84CA-2120D9DE9288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="465" windowWidth="29040" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="345" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="5" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCases!$A$9:$T$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCases!$A$9:$T$89</definedName>
     <definedName name="filtro" localSheetId="0">TestCases!$A$9:$S$89</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -1251,13 +1251,13 @@
     <t>2.16.840.1.113883.2.9.2.110.4.4.3ef6f06ee2145e043d78951fa763bda4494f40e89021bb5220992b438cf759d2.6ae9b446b0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>a499eba6c659a277</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.0790ca93f8b308251521d3054e27fd1cd541f3b90688f98e34e1557513d826fe.022ca9bbe1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>3f0e55f26a15964e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.3.1.4.4.ccc97c12937e3fc73a6418f78f3e901f13350ed72befb4e5d55235a88418afaf.97bbc59afe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1990,7 +1990,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B85" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2417,7 +2417,7 @@
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
       <c r="N13" s="15" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
@@ -5886,16 +5886,16 @@
       </c>
       <c r="E88" s="12"/>
       <c r="F88" s="13">
-        <v>45098</v>
+        <v>45097</v>
       </c>
       <c r="G88" s="14">
-        <v>45098.524108796293</v>
+        <v>45097.975266203706</v>
       </c>
       <c r="H88" s="14" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="I88" s="14" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="J88" s="15" t="s">
         <v>38</v>
@@ -15563,11 +15563,7 @@
       <c r="T709" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T91" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:T91">
-      <sortCondition ref="A9:A91"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A9:T89" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>

</xml_diff>

<commit_message>
modifiche a seguito di segnaalazione
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111NBSSRLXXXXX/NBS/networksanitario/v.4.10.106/report-checklist.xlsx
+++ b/GATEWAY/S1#111NBSSRLXXXXX/NBS/networksanitario/v.4.10.106/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.damiani\Desktop\it-fse-accreditamento\GATEWAY\S1#111NBSSRLXXXXX\NBS\networksanitario\v.4.10.106\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF6D1CA-620E-41A0-A0CC-B9735894049A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1003AB3-E90D-4B00-9C3E-A2AD4A5BE4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="465" windowWidth="29040" windowHeight="15855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="345" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
@@ -1442,12 +1442,6 @@
     <t>VALIDAZIONE_CDA2_RAD_CT0</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a1f91f2f4beb6bf12cb41f0df46c501aa5078fe9791c8395294a8e5440019d5e.df822295aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>5540af19836e6fac</t>
-  </si>
-  <si>
     <t>ac3d87cc1065c942</t>
   </si>
   <si>
@@ -1505,6 +1499,12 @@
   <si>
     <t>In caso di errore il processo applicativo prosegue ed il documento viene firmato. Eventuali verifiche, correzioni dei dati e re-invii vengono concordati/definiti con le singole aziende.
 Viene messo a disposizione dell'azienda una modalità di verifica dei documenti che hanno avuto errori di validazione da parte del gateway per poterli individuare e procedere alla correzione, firma e re-invio..</t>
+  </si>
+  <si>
+    <t>53ec8f7204459202</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a1f91f2f4beb6bf12cb41f0df46c501aa5078fe9791c8395294a8e5440019d5e.f4ba1c7a16^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2234,10 +2234,10 @@
   <dimension ref="A1:U736"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="G63" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B111" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="O67" sqref="O67"/>
+      <selection pane="bottomRight" activeCell="H114" sqref="H114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3024,7 +3024,7 @@
         <v>38</v>
       </c>
       <c r="P22" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q22" s="15"/>
       <c r="R22" s="16"/>
@@ -3056,7 +3056,7 @@
         <v>45105.520231481481</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I23" s="14" t="s">
         <v>66</v>
@@ -3078,7 +3078,7 @@
         <v>38</v>
       </c>
       <c r="P23" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q23" s="15"/>
       <c r="R23" s="16"/>
@@ -3274,7 +3274,7 @@
         <v>45105.52375</v>
       </c>
       <c r="H27" s="37" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I27" s="14" t="s">
         <v>66</v>
@@ -3296,7 +3296,7 @@
         <v>38</v>
       </c>
       <c r="P27" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q27" s="15"/>
       <c r="R27" s="16"/>
@@ -3723,7 +3723,7 @@
         <v>38</v>
       </c>
       <c r="P36" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q36" s="15"/>
       <c r="R36" s="16"/>
@@ -3967,7 +3967,7 @@
         <v>38</v>
       </c>
       <c r="P42" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q42" s="15"/>
       <c r="R42" s="16"/>
@@ -4021,7 +4021,7 @@
         <v>38</v>
       </c>
       <c r="P43" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q43" s="15"/>
       <c r="R43" s="16"/>
@@ -4075,7 +4075,7 @@
         <v>38</v>
       </c>
       <c r="P44" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q44" s="15"/>
       <c r="R44" s="16"/>
@@ -4129,7 +4129,7 @@
         <v>38</v>
       </c>
       <c r="P45" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q45" s="15"/>
       <c r="R45" s="16"/>
@@ -4161,10 +4161,10 @@
         <v>45105.604085648149</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="J46" s="15" t="s">
         <v>38</v>
@@ -4177,13 +4177,13 @@
         <v>38</v>
       </c>
       <c r="N46" s="15" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="O46" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P46" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q46" s="15"/>
       <c r="R46" s="16"/>
@@ -4367,10 +4367,10 @@
         <v>45105.675555555557</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J51" s="15" t="s">
         <v>38</v>
@@ -4383,13 +4383,13 @@
         <v>38</v>
       </c>
       <c r="N51" s="15" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="O51" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P51" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q51" s="15"/>
       <c r="R51" s="16"/>
@@ -4459,10 +4459,10 @@
         <v>45105.691793981481</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J53" s="15" t="s">
         <v>38</v>
@@ -4475,13 +4475,13 @@
         <v>38</v>
       </c>
       <c r="N53" s="15" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="O53" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P53" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q53" s="15"/>
       <c r="R53" s="16"/>
@@ -4514,7 +4514,7 @@
         <v>65</v>
       </c>
       <c r="K54" s="15" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
@@ -4551,10 +4551,10 @@
         <v>45105.717881944445</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J55" s="15" t="s">
         <v>38</v>
@@ -4567,13 +4567,13 @@
         <v>38</v>
       </c>
       <c r="N55" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="O55" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P55" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q55" s="15"/>
       <c r="R55" s="16"/>
@@ -4606,7 +4606,7 @@
         <v>65</v>
       </c>
       <c r="K56" s="15" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
@@ -4682,7 +4682,7 @@
         <v>65</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
@@ -5044,7 +5044,7 @@
         <v>38</v>
       </c>
       <c r="P67" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="Q67" s="15"/>
       <c r="R67" s="16"/>
@@ -5250,7 +5250,7 @@
         <v>38</v>
       </c>
       <c r="P72" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q72" s="15"/>
       <c r="R72" s="16"/>
@@ -5304,7 +5304,7 @@
         <v>38</v>
       </c>
       <c r="P73" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q73" s="15"/>
       <c r="R73" s="16"/>
@@ -5358,7 +5358,7 @@
         <v>38</v>
       </c>
       <c r="P74" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q74" s="15"/>
       <c r="R74" s="16"/>
@@ -5412,7 +5412,7 @@
         <v>38</v>
       </c>
       <c r="P75" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q75" s="15"/>
       <c r="R75" s="16"/>
@@ -5542,7 +5542,7 @@
         <v>38</v>
       </c>
       <c r="P78" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q78" s="15"/>
       <c r="R78" s="16"/>
@@ -5633,7 +5633,7 @@
         <v>38</v>
       </c>
       <c r="P80" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q80" s="15"/>
       <c r="R80" s="16"/>
@@ -5687,7 +5687,7 @@
         <v>38</v>
       </c>
       <c r="P81" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q81" s="15"/>
       <c r="R81" s="16"/>
@@ -5817,7 +5817,7 @@
         <v>38</v>
       </c>
       <c r="P84" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q84" s="15"/>
       <c r="R84" s="16"/>
@@ -5871,7 +5871,7 @@
         <v>38</v>
       </c>
       <c r="P85" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q85" s="15"/>
       <c r="R85" s="16"/>
@@ -5925,7 +5925,7 @@
         <v>38</v>
       </c>
       <c r="P86" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q86" s="15"/>
       <c r="R86" s="16"/>
@@ -5979,7 +5979,7 @@
         <v>38</v>
       </c>
       <c r="P87" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q87" s="15"/>
       <c r="R87" s="16"/>
@@ -6071,7 +6071,7 @@
         <v>38</v>
       </c>
       <c r="P89" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q89" s="15"/>
       <c r="R89" s="16"/>
@@ -6287,7 +6287,7 @@
         <v>38</v>
       </c>
       <c r="P94" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q94" s="15"/>
       <c r="R94" s="16"/>
@@ -6379,7 +6379,7 @@
         <v>38</v>
       </c>
       <c r="P96" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q96" s="15"/>
       <c r="R96" s="16"/>
@@ -6585,7 +6585,7 @@
         <v>38</v>
       </c>
       <c r="P101" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q101" s="15"/>
       <c r="R101" s="16"/>
@@ -6639,7 +6639,7 @@
         <v>38</v>
       </c>
       <c r="P102" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q102" s="15"/>
       <c r="R102" s="16"/>
@@ -6693,7 +6693,7 @@
         <v>38</v>
       </c>
       <c r="P103" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q103" s="15"/>
       <c r="R103" s="16"/>
@@ -6747,7 +6747,7 @@
         <v>38</v>
       </c>
       <c r="P104" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q104" s="15"/>
       <c r="R104" s="16"/>
@@ -6801,7 +6801,7 @@
         <v>38</v>
       </c>
       <c r="P105" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q105" s="15"/>
       <c r="R105" s="16"/>
@@ -6893,7 +6893,7 @@
         <v>38</v>
       </c>
       <c r="P107" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q107" s="15"/>
       <c r="R107" s="16"/>
@@ -6947,7 +6947,7 @@
         <v>38</v>
       </c>
       <c r="P108" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q108" s="15"/>
       <c r="R108" s="16"/>
@@ -7001,7 +7001,7 @@
         <v>38</v>
       </c>
       <c r="P109" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q109" s="15"/>
       <c r="R109" s="16"/>
@@ -7055,7 +7055,7 @@
         <v>38</v>
       </c>
       <c r="P110" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q110" s="15"/>
       <c r="R110" s="16"/>
@@ -7147,7 +7147,7 @@
         <v>38</v>
       </c>
       <c r="P112" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q112" s="15"/>
       <c r="R112" s="16"/>
@@ -7220,13 +7220,13 @@
         <v>45105</v>
       </c>
       <c r="G114" s="14">
-        <v>45105.511412037034</v>
+        <v>45105.704733796294</v>
       </c>
       <c r="H114" s="14" t="s">
-        <v>386</v>
+        <v>404</v>
       </c>
       <c r="I114" s="14" t="s">
-        <v>385</v>
+        <v>405</v>
       </c>
       <c r="J114" s="15" t="s">
         <v>38</v>
@@ -7239,7 +7239,7 @@
         <v>38</v>
       </c>
       <c r="P114" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Q114" s="15"/>
       <c r="R114" s="16"/>

</xml_diff>

<commit_message>
Modifica case test per errore
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111NBSSRLXXXXX/NBS/networksanitario/v.4.10.106/report-checklist.xlsx
+++ b/GATEWAY/S1#111NBSSRLXXXXX/NBS/networksanitario/v.4.10.106/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.damiani\Desktop\it-fse-accreditamento\GATEWAY\S1#111NBSSRLXXXXX\NBS\networksanitario\v.4.10.106\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.daversa\Desktop\patch_in_lavorazione\fes20\it-fse-accreditamento\GATEWAY\S1#111NBSSRLXXXXX\NBS\networksanitario\v.4.10.106\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1003AB3-E90D-4B00-9C3E-A2AD4A5BE4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA47F4C9-9902-4042-AFF7-D993E3263DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="345" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
@@ -992,12 +992,6 @@
     <t>422-[ERRORE-b57| Sotto-sezione Allergie: entry/act/entryRelationship/observation deve contenere almeno un elemento 'participant']</t>
   </si>
   <si>
-    <t>4640452d69354dea</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.bd5a2f263e4d844d56c6878edaaee87b01ffd6ab86c32e4959f1830291c133db.9f474dd745^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>422-[ERRORE-30| L'elemento ClinicalDocument/legalAuthenticator/signatureCode deve essere valorizzato con il codice \"S\</t>
   </si>
   <si>
@@ -1198,12 +1192,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.110.4.4.e5616e1f35fd0b1bfff0708b6850769a84d649c4cc4aa9af11d89158d2a7e9a4.3cb534736f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>5a717427df3d9dda</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.b9e07f30eb2389c65055dd9fb195bd1da6336c32cfa24aeac56bb12a73e8eb48.98e9c9a136^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>c9403b812b4a9536</t>
@@ -1505,6 +1493,18 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a1f91f2f4beb6bf12cb41f0df46c501aa5078fe9791c8395294a8e5440019d5e.f4ba1c7a16^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.bd5a2f263e4d844d56c6878edaaee87b01ffd6ab86c32e4959f1830291c133db.344ea3cd45^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>9ebe8a49a78e80ef</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.110.4.4.b9e07f30eb2389c65055dd9fb195bd1da6336c32cfa24aeac56bb12a73e8eb48.093d4228fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ae6aa4deccc52eba</t>
   </si>
 </sst>
 </file>
@@ -2234,10 +2234,10 @@
   <dimension ref="A1:U736"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B111" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B100" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H114" sqref="H114"/>
+      <selection pane="bottomRight" activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2514,10 +2514,10 @@
         <v>45104.40084490741</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J10" s="15" t="s">
         <v>38</v>
@@ -2562,10 +2562,10 @@
         <v>45104.402025462965</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>38</v>
@@ -2610,10 +2610,10 @@
         <v>45104.403078703705</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J12" s="20" t="s">
         <v>38</v>
@@ -2664,7 +2664,7 @@
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
       <c r="N13" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
@@ -2683,13 +2683,13 @@
         <v>25</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="14"/>
@@ -2721,13 +2721,13 @@
         <v>25</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="E15" s="34" t="s">
         <v>333</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>336</v>
-      </c>
-      <c r="E15" s="34" t="s">
-        <v>337</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="14"/>
@@ -2759,13 +2759,13 @@
         <v>25</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="14"/>
@@ -2797,13 +2797,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="14"/>
@@ -3002,7 +3002,7 @@
         <v>45104.406759259262</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I22" s="14" t="s">
         <v>66</v>
@@ -3024,7 +3024,7 @@
         <v>38</v>
       </c>
       <c r="P22" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q22" s="15"/>
       <c r="R22" s="16"/>
@@ -3041,13 +3041,13 @@
         <v>25</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F23" s="13">
         <v>45105</v>
@@ -3056,7 +3056,7 @@
         <v>45105.520231481481</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="I23" s="14" t="s">
         <v>66</v>
@@ -3078,7 +3078,7 @@
         <v>38</v>
       </c>
       <c r="P23" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q23" s="15"/>
       <c r="R23" s="16"/>
@@ -3110,7 +3110,7 @@
         <v>45104.407858796294</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I24" s="14" t="s">
         <v>66</v>
@@ -3164,7 +3164,7 @@
         <v>45104.410115740742</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I25" s="14" t="s">
         <v>66</v>
@@ -3218,7 +3218,7 @@
         <v>45104.412164351852</v>
       </c>
       <c r="H26" s="37" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I26" s="14" t="s">
         <v>66</v>
@@ -3259,13 +3259,13 @@
         <v>25</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F27" s="13">
         <v>45105</v>
@@ -3274,7 +3274,7 @@
         <v>45105.52375</v>
       </c>
       <c r="H27" s="37" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="I27" s="14" t="s">
         <v>66</v>
@@ -3296,7 +3296,7 @@
         <v>38</v>
       </c>
       <c r="P27" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q27" s="15"/>
       <c r="R27" s="16"/>
@@ -3328,7 +3328,7 @@
         <v>45104.412905092591</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I28" s="14" t="s">
         <v>66</v>
@@ -3382,7 +3382,7 @@
         <v>45104.413842592592</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I29" s="14" t="s">
         <v>66</v>
@@ -3473,10 +3473,10 @@
         <v>25</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>183</v>
@@ -3626,7 +3626,7 @@
         <v>65</v>
       </c>
       <c r="K34" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
@@ -3701,10 +3701,10 @@
         <v>45104.416215277779</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J36" s="15" t="s">
         <v>38</v>
@@ -3723,7 +3723,7 @@
         <v>38</v>
       </c>
       <c r="P36" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q36" s="15"/>
       <c r="R36" s="16"/>
@@ -3945,10 +3945,10 @@
         <v>45104.426342592589</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J42" s="36" t="s">
         <v>38</v>
@@ -3967,7 +3967,7 @@
         <v>38</v>
       </c>
       <c r="P42" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q42" s="15"/>
       <c r="R42" s="16"/>
@@ -3999,10 +3999,10 @@
         <v>45104.427581018521</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J43" s="15" t="s">
         <v>38</v>
@@ -4021,7 +4021,7 @@
         <v>38</v>
       </c>
       <c r="P43" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q43" s="15"/>
       <c r="R43" s="16"/>
@@ -4053,10 +4053,10 @@
         <v>45104.428587962961</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J44" s="15" t="s">
         <v>38</v>
@@ -4075,7 +4075,7 @@
         <v>38</v>
       </c>
       <c r="P44" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q44" s="15"/>
       <c r="R44" s="16"/>
@@ -4107,10 +4107,10 @@
         <v>45104.429884259262</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J45" s="15" t="s">
         <v>38</v>
@@ -4123,13 +4123,13 @@
         <v>38</v>
       </c>
       <c r="N45" s="15" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="O45" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P45" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q45" s="15"/>
       <c r="R45" s="16"/>
@@ -4146,13 +4146,13 @@
         <v>25</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="F46" s="13">
         <v>45105</v>
@@ -4161,10 +4161,10 @@
         <v>45105.604085648149</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="J46" s="15" t="s">
         <v>38</v>
@@ -4177,13 +4177,13 @@
         <v>38</v>
       </c>
       <c r="N46" s="15" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="O46" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P46" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q46" s="15"/>
       <c r="R46" s="16"/>
@@ -4200,13 +4200,13 @@
         <v>25</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F47" s="13"/>
       <c r="G47" s="14"/>
@@ -4238,13 +4238,13 @@
         <v>25</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F48" s="13"/>
       <c r="G48" s="14"/>
@@ -4276,13 +4276,13 @@
         <v>25</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F49" s="13"/>
       <c r="G49" s="14"/>
@@ -4314,13 +4314,13 @@
         <v>25</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="14"/>
@@ -4352,13 +4352,13 @@
         <v>25</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="F51" s="13">
         <v>45105</v>
@@ -4367,10 +4367,10 @@
         <v>45105.675555555557</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="J51" s="15" t="s">
         <v>38</v>
@@ -4383,13 +4383,13 @@
         <v>38</v>
       </c>
       <c r="N51" s="15" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="O51" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P51" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q51" s="15"/>
       <c r="R51" s="16"/>
@@ -4406,13 +4406,13 @@
         <v>25</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F52" s="13"/>
       <c r="G52" s="14"/>
@@ -4444,13 +4444,13 @@
         <v>25</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F53" s="13">
         <v>45105</v>
@@ -4459,10 +4459,10 @@
         <v>45105.691793981481</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="J53" s="15" t="s">
         <v>38</v>
@@ -4475,13 +4475,13 @@
         <v>38</v>
       </c>
       <c r="N53" s="15" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="O53" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P53" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q53" s="15"/>
       <c r="R53" s="16"/>
@@ -4498,13 +4498,13 @@
         <v>25</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F54" s="13"/>
       <c r="G54" s="14"/>
@@ -4514,7 +4514,7 @@
         <v>65</v>
       </c>
       <c r="K54" s="15" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
@@ -4536,13 +4536,13 @@
         <v>25</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F55" s="13">
         <v>45105</v>
@@ -4551,10 +4551,10 @@
         <v>45105.717881944445</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="J55" s="15" t="s">
         <v>38</v>
@@ -4567,13 +4567,13 @@
         <v>38</v>
       </c>
       <c r="N55" s="15" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="O55" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P55" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q55" s="15"/>
       <c r="R55" s="16"/>
@@ -4590,13 +4590,13 @@
         <v>25</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F56" s="13"/>
       <c r="G56" s="14"/>
@@ -4606,7 +4606,7 @@
         <v>65</v>
       </c>
       <c r="K56" s="15" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
@@ -4628,13 +4628,13 @@
         <v>25</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="F57" s="13"/>
       <c r="G57" s="14"/>
@@ -4666,13 +4666,13 @@
         <v>25</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F58" s="13"/>
       <c r="G58" s="14"/>
@@ -4682,7 +4682,7 @@
         <v>65</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
@@ -4704,13 +4704,13 @@
         <v>25</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F59" s="13"/>
       <c r="G59" s="14"/>
@@ -4742,13 +4742,13 @@
         <v>25</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="F60" s="13"/>
       <c r="G60" s="14"/>
@@ -4780,13 +4780,13 @@
         <v>25</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F61" s="13"/>
       <c r="G61" s="14"/>
@@ -4818,13 +4818,13 @@
         <v>25</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="F62" s="13"/>
       <c r="G62" s="14"/>
@@ -4856,13 +4856,13 @@
         <v>25</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="F63" s="13"/>
       <c r="G63" s="14"/>
@@ -4894,13 +4894,13 @@
         <v>25</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="F64" s="13"/>
       <c r="G64" s="14"/>
@@ -4948,7 +4948,7 @@
         <v>65</v>
       </c>
       <c r="K65" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="L65" s="15"/>
       <c r="M65" s="15"/>
@@ -5023,10 +5023,10 @@
         <v>45104.434178240743</v>
       </c>
       <c r="H67" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="I67" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J67" s="15" t="s">
         <v>38</v>
@@ -5044,7 +5044,7 @@
         <v>38</v>
       </c>
       <c r="P67" s="15" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="Q67" s="15"/>
       <c r="R67" s="16"/>
@@ -5228,10 +5228,10 @@
         <v>45104.435486111113</v>
       </c>
       <c r="H72" s="37" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I72" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J72" s="15" t="s">
         <v>38</v>
@@ -5250,7 +5250,7 @@
         <v>38</v>
       </c>
       <c r="P72" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q72" s="15"/>
       <c r="R72" s="16"/>
@@ -5282,10 +5282,10 @@
         <v>45104.436909722222</v>
       </c>
       <c r="H73" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I73" s="14" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J73" s="15" t="s">
         <v>38</v>
@@ -5304,7 +5304,7 @@
         <v>38</v>
       </c>
       <c r="P73" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q73" s="15"/>
       <c r="R73" s="16"/>
@@ -5336,7 +5336,7 @@
         <v>45104.438668981478</v>
       </c>
       <c r="H74" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I74" s="14" t="s">
         <v>144</v>
@@ -5358,7 +5358,7 @@
         <v>38</v>
       </c>
       <c r="P74" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q74" s="15"/>
       <c r="R74" s="16"/>
@@ -5390,10 +5390,10 @@
         <v>45104.439479166664</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I75" s="14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J75" s="15" t="s">
         <v>38</v>
@@ -5412,7 +5412,7 @@
         <v>38</v>
       </c>
       <c r="P75" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q75" s="15"/>
       <c r="R75" s="16"/>
@@ -5520,10 +5520,10 @@
         <v>45104.442962962959</v>
       </c>
       <c r="H78" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I78" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J78" s="15" t="s">
         <v>38</v>
@@ -5542,7 +5542,7 @@
         <v>38</v>
       </c>
       <c r="P78" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q78" s="15"/>
       <c r="R78" s="16"/>
@@ -5611,10 +5611,10 @@
         <v>45104.443761574075</v>
       </c>
       <c r="H80" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I80" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J80" s="15" t="s">
         <v>38</v>
@@ -5633,7 +5633,7 @@
         <v>38</v>
       </c>
       <c r="P80" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q80" s="15"/>
       <c r="R80" s="16"/>
@@ -5665,10 +5665,10 @@
         <v>45104.444768518515</v>
       </c>
       <c r="H81" s="14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I81" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J81" s="15" t="s">
         <v>38</v>
@@ -5687,7 +5687,7 @@
         <v>38</v>
       </c>
       <c r="P81" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q81" s="15"/>
       <c r="R81" s="16"/>
@@ -5795,10 +5795,10 @@
         <v>45104.445601851854</v>
       </c>
       <c r="H84" s="14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I84" s="38" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J84" s="15" t="s">
         <v>38</v>
@@ -5817,7 +5817,7 @@
         <v>38</v>
       </c>
       <c r="P84" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q84" s="15"/>
       <c r="R84" s="16"/>
@@ -5849,10 +5849,10 @@
         <v>45104.446585648147</v>
       </c>
       <c r="H85" s="14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I85" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J85" s="15" t="s">
         <v>38</v>
@@ -5871,7 +5871,7 @@
         <v>38</v>
       </c>
       <c r="P85" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q85" s="15"/>
       <c r="R85" s="16"/>
@@ -5903,10 +5903,10 @@
         <v>45104.447384259256</v>
       </c>
       <c r="H86" s="14" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I86" s="14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J86" s="15" t="s">
         <v>38</v>
@@ -5925,7 +5925,7 @@
         <v>38</v>
       </c>
       <c r="P86" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q86" s="15"/>
       <c r="R86" s="16"/>
@@ -5957,10 +5957,10 @@
         <v>45104.449189814812</v>
       </c>
       <c r="H87" s="14" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I87" s="14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J87" s="15" t="s">
         <v>38</v>
@@ -5979,7 +5979,7 @@
         <v>38</v>
       </c>
       <c r="P87" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q87" s="15"/>
       <c r="R87" s="16"/>
@@ -6049,10 +6049,10 @@
         <v>45104.450011574074</v>
       </c>
       <c r="H89" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I89" s="14" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J89" s="15" t="s">
         <v>38</v>
@@ -6071,7 +6071,7 @@
         <v>38</v>
       </c>
       <c r="P89" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q89" s="15"/>
       <c r="R89" s="16"/>
@@ -6103,10 +6103,10 @@
         <v>45104.450856481482</v>
       </c>
       <c r="H90" s="14" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I90" s="14" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J90" s="15" t="s">
         <v>38</v>
@@ -6265,10 +6265,10 @@
         <v>45104.451840277776</v>
       </c>
       <c r="H94" s="14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I94" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J94" s="15" t="s">
         <v>38</v>
@@ -6287,7 +6287,7 @@
         <v>38</v>
       </c>
       <c r="P94" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q94" s="15"/>
       <c r="R94" s="16"/>
@@ -6351,16 +6351,16 @@
         <v>213</v>
       </c>
       <c r="F96" s="13">
-        <v>45104</v>
+        <v>45111</v>
       </c>
       <c r="G96" s="14">
-        <v>45104.703912037039</v>
+        <v>45111.63380787037</v>
       </c>
       <c r="H96" s="14" t="s">
-        <v>246</v>
+        <v>403</v>
       </c>
       <c r="I96" s="14" t="s">
-        <v>247</v>
+        <v>402</v>
       </c>
       <c r="J96" s="15" t="s">
         <v>38</v>
@@ -6379,7 +6379,7 @@
         <v>38</v>
       </c>
       <c r="P96" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q96" s="15"/>
       <c r="R96" s="16"/>
@@ -6563,10 +6563,10 @@
         <v>45104.454525462963</v>
       </c>
       <c r="H101" s="14" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I101" s="14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J101" s="15" t="s">
         <v>38</v>
@@ -6585,7 +6585,7 @@
         <v>38</v>
       </c>
       <c r="P101" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q101" s="15"/>
       <c r="R101" s="16"/>
@@ -6617,10 +6617,10 @@
         <v>45104.455439814818</v>
       </c>
       <c r="H102" s="14" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I102" s="14" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J102" s="15" t="s">
         <v>38</v>
@@ -6639,7 +6639,7 @@
         <v>38</v>
       </c>
       <c r="P102" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q102" s="15"/>
       <c r="R102" s="16"/>
@@ -6671,10 +6671,10 @@
         <v>45104.456284722219</v>
       </c>
       <c r="H103" s="14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I103" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J103" s="15" t="s">
         <v>38</v>
@@ -6693,7 +6693,7 @@
         <v>38</v>
       </c>
       <c r="P103" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q103" s="15"/>
       <c r="R103" s="16"/>
@@ -6725,10 +6725,10 @@
         <v>45104.457465277781</v>
       </c>
       <c r="H104" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I104" s="14" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J104" s="15" t="s">
         <v>38</v>
@@ -6747,7 +6747,7 @@
         <v>38</v>
       </c>
       <c r="P104" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q104" s="15"/>
       <c r="R104" s="16"/>
@@ -6756,57 +6756,57 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="19">
+    <row r="105" spans="1:20" s="33" customFormat="1" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="23">
         <v>162</v>
       </c>
-      <c r="B105" s="11" t="s">
+      <c r="B105" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C105" s="11" t="s">
+      <c r="C105" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="D105" s="11" t="s">
+      <c r="D105" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="E105" s="12" t="s">
+      <c r="E105" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="F105" s="13">
+      <c r="F105" s="26">
         <v>45104</v>
       </c>
-      <c r="G105" s="14">
-        <v>45104.463773148149</v>
-      </c>
-      <c r="H105" s="14" t="s">
-        <v>315</v>
-      </c>
-      <c r="I105" s="14" t="s">
-        <v>316</v>
-      </c>
-      <c r="J105" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="K105" s="15"/>
-      <c r="L105" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="M105" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="N105" s="15" t="s">
+      <c r="G105" s="27">
+        <v>45104.772928240738</v>
+      </c>
+      <c r="H105" s="27" t="s">
+        <v>405</v>
+      </c>
+      <c r="I105" s="27" t="s">
+        <v>404</v>
+      </c>
+      <c r="J105" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="K105" s="29"/>
+      <c r="L105" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="M105" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="N105" s="29" t="s">
         <v>240</v>
       </c>
-      <c r="O105" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="P105" s="15" t="s">
-        <v>402</v>
-      </c>
-      <c r="Q105" s="15"/>
-      <c r="R105" s="16"/>
-      <c r="S105" s="17"/>
-      <c r="T105" s="18" t="s">
+      <c r="O105" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="P105" s="29" t="s">
+        <v>398</v>
+      </c>
+      <c r="Q105" s="29"/>
+      <c r="R105" s="30"/>
+      <c r="S105" s="31"/>
+      <c r="T105" s="32" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6871,10 +6871,10 @@
         <v>45104.464988425927</v>
       </c>
       <c r="H107" s="14" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="I107" s="14" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="J107" s="15" t="s">
         <v>38</v>
@@ -6893,7 +6893,7 @@
         <v>38</v>
       </c>
       <c r="P107" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q107" s="15"/>
       <c r="R107" s="16"/>
@@ -6925,10 +6925,10 @@
         <v>45104.773680555554</v>
       </c>
       <c r="H108" s="14" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="I108" s="14" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="J108" s="15" t="s">
         <v>38</v>
@@ -6947,7 +6947,7 @@
         <v>38</v>
       </c>
       <c r="P108" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q108" s="15"/>
       <c r="R108" s="16"/>
@@ -6979,10 +6979,10 @@
         <v>45104.774641203701</v>
       </c>
       <c r="H109" s="14" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="I109" s="14" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="J109" s="15" t="s">
         <v>38</v>
@@ -7001,7 +7001,7 @@
         <v>38</v>
       </c>
       <c r="P109" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q109" s="15"/>
       <c r="R109" s="16"/>
@@ -7033,10 +7033,10 @@
         <v>45104.775740740741</v>
       </c>
       <c r="H110" s="14" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="I110" s="14" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="J110" s="15" t="s">
         <v>38</v>
@@ -7055,7 +7055,7 @@
         <v>38</v>
       </c>
       <c r="P110" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q110" s="15"/>
       <c r="R110" s="16"/>
@@ -7116,7 +7116,7 @@
         <v>210</v>
       </c>
       <c r="E112" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F112" s="13">
         <v>45104</v>
@@ -7125,10 +7125,10 @@
         <v>45104.776620370372</v>
       </c>
       <c r="H112" s="14" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="I112" s="14" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="J112" s="15" t="s">
         <v>38</v>
@@ -7141,13 +7141,13 @@
         <v>38</v>
       </c>
       <c r="N112" s="15" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O112" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P112" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q112" s="15"/>
       <c r="R112" s="16"/>
@@ -7167,7 +7167,7 @@
         <v>24</v>
       </c>
       <c r="D113" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E113" s="12"/>
       <c r="F113" s="13">
@@ -7177,10 +7177,10 @@
         <v>45104.777511574073</v>
       </c>
       <c r="H113" s="14" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="I113" s="14" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="J113" s="15" t="s">
         <v>38</v>
@@ -7210,10 +7210,10 @@
         <v>25</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D114" s="11" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E114" s="12"/>
       <c r="F114" s="13">
@@ -7223,10 +7223,10 @@
         <v>45105.704733796294</v>
       </c>
       <c r="H114" s="14" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="I114" s="14" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="J114" s="15" t="s">
         <v>38</v>
@@ -7239,7 +7239,7 @@
         <v>38</v>
       </c>
       <c r="P114" s="15" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Q114" s="15"/>
       <c r="R114" s="16"/>
@@ -7259,7 +7259,7 @@
         <v>87</v>
       </c>
       <c r="D115" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E115" s="12"/>
       <c r="F115" s="13">
@@ -7269,10 +7269,10 @@
         <v>45104.778263888889</v>
       </c>
       <c r="H115" s="14" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="I115" s="14" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="J115" s="15" t="s">
         <v>38</v>
@@ -7305,7 +7305,7 @@
         <v>174</v>
       </c>
       <c r="D116" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E116" s="12"/>
       <c r="F116" s="13">
@@ -7315,10 +7315,10 @@
         <v>45104.779027777775</v>
       </c>
       <c r="H116" s="14" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="I116" s="14" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="J116" s="15" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
correzzione a seguito di segnalazione
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111NBSSRLXXXXX/NBS/networksanitario/v.4.10.106/report-checklist.xlsx
+++ b/GATEWAY/S1#111NBSSRLXXXXX/NBS/networksanitario/v.4.10.106/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.daversa\Desktop\patch_in_lavorazione\fes20\it-fse-accreditamento\GATEWAY\S1#111NBSSRLXXXXX\NBS\networksanitario\v.4.10.106\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.damiani\Desktop\it-fse-accreditamento\GATEWAY\S1#111NBSSRLXXXXX\NBS\networksanitario\v.4.10.106\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA47F4C9-9902-4042-AFF7-D993E3263DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E1DA6B-293F-4058-92FE-2E56117CC7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="345" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="406">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -372,9 +372,6 @@
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>IL SERVIZIO MOSTRA UN MESSAGGIO DI ERRORE INTERNO E TENTA IL REINVIO</t>
-  </si>
-  <si>
     <t>403:Il campo action_id non è corretto</t>
   </si>
   <si>
@@ -601,11 +598,6 @@
   </si>
   <si>
     <t>403-Campo token JWT non valido,Il campo purpose_of_use non è valorizzato</t>
-  </si>
-  <si>
-    <t>Attenzione!
-Il servizio di validazione ha impiegato troppo tempo a rispondere. 
-Tentare di nuovo il processo di validazione?</t>
   </si>
   <si>
     <t>Il software esegue controlli di congruneza del  CF e correttezza impostandolo in maiuscolo</t>
@@ -1505,6 +1497,15 @@
   </si>
   <si>
     <t>ae6aa4deccc52eba</t>
+  </si>
+  <si>
+    <t>In caso di errore il processo applicativo prosegue ed il documento viene firmato. Eventuali verifiche, correzioni dei dati e re-invii vengono concordati/definiti con le singole aziende.
+Viene messo a disposizione dell'azienda una modalità di verifica dei documenti che hanno avuto errori di validazione da parte del gateway per poterli individuare e procedere alla correzione, firma e re-invio.?</t>
+  </si>
+  <si>
+    <t>Attenzione!
+Il servizio di validazione ha impiegato troppo tempo a rispondere. 
+Procedere alla firma?</t>
   </si>
 </sst>
 </file>
@@ -2231,13 +2232,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:U736"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B100" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B106" sqref="B106"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2281,7 +2283,7 @@
       </c>
       <c r="B2" s="46"/>
       <c r="C2" s="47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2" s="46"/>
       <c r="F2" s="3"/>
@@ -2306,7 +2308,7 @@
       </c>
       <c r="B3" s="49"/>
       <c r="C3" s="54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="55"/>
       <c r="F3" s="3"/>
@@ -2329,7 +2331,7 @@
       <c r="A4" s="50"/>
       <c r="B4" s="51"/>
       <c r="C4" s="54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="55"/>
       <c r="E4" s="2"/>
@@ -2353,7 +2355,7 @@
       <c r="A5" s="52"/>
       <c r="B5" s="53"/>
       <c r="C5" s="54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="55"/>
       <c r="F5" s="3"/>
@@ -2491,7 +2493,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>6</v>
       </c>
@@ -2514,10 +2516,10 @@
         <v>45104.40084490741</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J10" s="15" t="s">
         <v>38</v>
@@ -2539,7 +2541,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>7</v>
       </c>
@@ -2562,10 +2564,10 @@
         <v>45104.402025462965</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>38</v>
@@ -2587,7 +2589,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>8</v>
       </c>
@@ -2610,10 +2612,10 @@
         <v>45104.403078703705</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J12" s="20" t="s">
         <v>38</v>
@@ -2635,7 +2637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>9</v>
       </c>
@@ -2659,12 +2661,12 @@
         <v>65</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
       <c r="N13" s="15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
@@ -2675,7 +2677,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="76.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>11</v>
       </c>
@@ -2683,13 +2685,13 @@
         <v>25</v>
       </c>
       <c r="C14" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="E14" s="34" t="s">
         <v>329</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>330</v>
-      </c>
-      <c r="E14" s="34" t="s">
-        <v>331</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="14"/>
@@ -2699,7 +2701,7 @@
         <v>65</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
@@ -2713,7 +2715,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="76.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>12</v>
       </c>
@@ -2721,13 +2723,13 @@
         <v>25</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="14"/>
@@ -2737,7 +2739,7 @@
         <v>65</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
@@ -2751,7 +2753,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="76.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>13</v>
       </c>
@@ -2759,13 +2761,13 @@
         <v>25</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D16" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="E16" s="34" t="s">
         <v>334</v>
-      </c>
-      <c r="E16" s="34" t="s">
-        <v>336</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="14"/>
@@ -2775,7 +2777,7 @@
         <v>65</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
@@ -2789,7 +2791,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="76.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>14</v>
       </c>
@@ -2797,13 +2799,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D17" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="E17" s="34" t="s">
         <v>335</v>
-      </c>
-      <c r="E17" s="34" t="s">
-        <v>337</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="14"/>
@@ -2813,7 +2815,7 @@
         <v>65</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
@@ -2827,7 +2829,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="105" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>24</v>
       </c>
@@ -2835,13 +2837,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="E18" s="34" t="s">
         <v>88</v>
-      </c>
-      <c r="E18" s="34" t="s">
-        <v>89</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="14"/>
@@ -2851,7 +2853,7 @@
         <v>65</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
@@ -2865,7 +2867,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="105" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>25</v>
       </c>
@@ -2873,13 +2875,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="34" t="s">
         <v>90</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>91</v>
       </c>
       <c r="F19" s="13"/>
       <c r="G19" s="14"/>
@@ -2889,7 +2891,7 @@
         <v>65</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
@@ -2903,7 +2905,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="105" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <v>26</v>
       </c>
@@ -2911,13 +2913,13 @@
         <v>25</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D20" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="34" t="s">
         <v>92</v>
-      </c>
-      <c r="E20" s="34" t="s">
-        <v>93</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="14"/>
@@ -2927,7 +2929,7 @@
         <v>65</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
@@ -2941,7 +2943,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="105" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19">
         <v>27</v>
       </c>
@@ -2949,13 +2951,13 @@
         <v>25</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="34" t="s">
         <v>94</v>
-      </c>
-      <c r="E21" s="34" t="s">
-        <v>95</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="14"/>
@@ -2965,7 +2967,7 @@
         <v>65</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
@@ -2979,7 +2981,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="225.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
         <v>29</v>
       </c>
@@ -3002,7 +3004,7 @@
         <v>45104.406759259262</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I22" s="14" t="s">
         <v>66</v>
@@ -3018,13 +3020,13 @@
         <v>38</v>
       </c>
       <c r="N22" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O22" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P22" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q22" s="15"/>
       <c r="R22" s="16"/>
@@ -3033,7 +3035,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="117.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="117.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>31</v>
       </c>
@@ -3041,13 +3043,13 @@
         <v>25</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F23" s="13">
         <v>45105</v>
@@ -3056,7 +3058,7 @@
         <v>45105.520231481481</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="I23" s="14" t="s">
         <v>66</v>
@@ -3072,13 +3074,13 @@
         <v>38</v>
       </c>
       <c r="N23" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O23" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P23" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q23" s="15"/>
       <c r="R23" s="16"/>
@@ -3087,7 +3089,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="156" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="156" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>32</v>
       </c>
@@ -3095,13 +3097,13 @@
         <v>25</v>
       </c>
       <c r="C24" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>174</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>175</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>176</v>
       </c>
       <c r="F24" s="13">
         <v>45104</v>
@@ -3110,7 +3112,7 @@
         <v>45104.407858796294</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I24" s="14" t="s">
         <v>66</v>
@@ -3126,13 +3128,13 @@
         <v>38</v>
       </c>
       <c r="N24" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O24" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P24" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q24" s="15"/>
       <c r="R24" s="16"/>
@@ -3141,7 +3143,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="150" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>35</v>
       </c>
@@ -3149,13 +3151,13 @@
         <v>25</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F25" s="13">
         <v>45104</v>
@@ -3164,7 +3166,7 @@
         <v>45104.410115740742</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I25" s="14" t="s">
         <v>66</v>
@@ -3180,13 +3182,13 @@
         <v>38</v>
       </c>
       <c r="N25" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O25" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P25" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q25" s="15"/>
       <c r="R25" s="16"/>
@@ -3195,7 +3197,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>37</v>
       </c>
@@ -3218,7 +3220,7 @@
         <v>45104.412164351852</v>
       </c>
       <c r="H26" s="37" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I26" s="14" t="s">
         <v>66</v>
@@ -3234,24 +3236,24 @@
         <v>38</v>
       </c>
       <c r="N26" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O26" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P26" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q26" s="15"/>
       <c r="R26" s="16"/>
       <c r="S26" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T26" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="136.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>39</v>
       </c>
@@ -3259,13 +3261,13 @@
         <v>25</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F27" s="13">
         <v>45105</v>
@@ -3274,7 +3276,7 @@
         <v>45105.52375</v>
       </c>
       <c r="H27" s="37" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I27" s="14" t="s">
         <v>66</v>
@@ -3290,13 +3292,13 @@
         <v>38</v>
       </c>
       <c r="N27" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O27" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P27" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q27" s="15"/>
       <c r="R27" s="16"/>
@@ -3305,7 +3307,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="110.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>40</v>
       </c>
@@ -3313,13 +3315,13 @@
         <v>25</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F28" s="13">
         <v>45104</v>
@@ -3328,7 +3330,7 @@
         <v>45104.412905092591</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I28" s="14" t="s">
         <v>66</v>
@@ -3344,13 +3346,13 @@
         <v>38</v>
       </c>
       <c r="N28" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="O28" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P28" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q28" s="15"/>
       <c r="R28" s="16"/>
@@ -3359,7 +3361,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="87.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
         <v>43</v>
       </c>
@@ -3367,13 +3369,13 @@
         <v>25</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F29" s="13">
         <v>45104</v>
@@ -3382,7 +3384,7 @@
         <v>45104.413842592592</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I29" s="14" t="s">
         <v>66</v>
@@ -3398,24 +3400,24 @@
         <v>38</v>
       </c>
       <c r="N29" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O29" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P29" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q29" s="15"/>
       <c r="R29" s="16"/>
       <c r="S29" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T29" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19">
         <v>45</v>
       </c>
@@ -3429,7 +3431,7 @@
         <v>39</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F30" s="13">
         <v>45104</v>
@@ -3450,13 +3452,13 @@
         <v>38</v>
       </c>
       <c r="N30" s="15" t="s">
-        <v>137</v>
+        <v>405</v>
       </c>
       <c r="O30" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P30" s="15" t="s">
-        <v>67</v>
+        <v>404</v>
       </c>
       <c r="Q30" s="20"/>
       <c r="R30" s="21"/>
@@ -3473,13 +3475,13 @@
         <v>25</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F31" s="13">
         <v>45105</v>
@@ -3489,13 +3491,25 @@
       </c>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
-      <c r="J31" s="15"/>
+      <c r="J31" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
+      <c r="L31" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="M31" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N31" s="15" t="s">
+        <v>405</v>
+      </c>
+      <c r="O31" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="P31" s="15" t="s">
+        <v>404</v>
+      </c>
       <c r="Q31" s="20"/>
       <c r="R31" s="40"/>
       <c r="S31" s="41"/>
@@ -3511,13 +3525,13 @@
         <v>25</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F32" s="13">
         <v>45104</v>
@@ -3538,13 +3552,13 @@
         <v>38</v>
       </c>
       <c r="N32" s="15" t="s">
-        <v>137</v>
+        <v>405</v>
       </c>
       <c r="O32" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P32" s="15" t="s">
-        <v>67</v>
+        <v>404</v>
       </c>
       <c r="Q32" s="20"/>
       <c r="R32" s="40"/>
@@ -3561,13 +3575,13 @@
         <v>25</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F33" s="13">
         <v>45104</v>
@@ -3588,13 +3602,13 @@
         <v>38</v>
       </c>
       <c r="N33" s="15" t="s">
-        <v>137</v>
+        <v>405</v>
       </c>
       <c r="O33" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P33" s="15" t="s">
-        <v>67</v>
+        <v>404</v>
       </c>
       <c r="Q33" s="20"/>
       <c r="S33" s="21"/>
@@ -3602,7 +3616,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
         <v>63</v>
       </c>
@@ -3626,7 +3640,7 @@
         <v>65</v>
       </c>
       <c r="K34" s="15" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
@@ -3640,7 +3654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="19">
         <v>64</v>
       </c>
@@ -3664,7 +3678,7 @@
         <v>65</v>
       </c>
       <c r="K35" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
@@ -3678,7 +3692,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="225.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19">
         <v>65</v>
       </c>
@@ -3689,7 +3703,7 @@
         <v>24</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>44</v>
@@ -3701,10 +3715,10 @@
         <v>45104.416215277779</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J36" s="15" t="s">
         <v>38</v>
@@ -3717,13 +3731,13 @@
         <v>38</v>
       </c>
       <c r="N36" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O36" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P36" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q36" s="15"/>
       <c r="R36" s="16"/>
@@ -3732,7 +3746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:20" s="33" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" s="33" customFormat="1" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="23">
         <v>66</v>
       </c>
@@ -3756,7 +3770,7 @@
         <v>65</v>
       </c>
       <c r="K37" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L37" s="29"/>
       <c r="M37" s="29"/>
@@ -3770,7 +3784,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19">
         <v>67</v>
       </c>
@@ -3794,7 +3808,7 @@
         <v>65</v>
       </c>
       <c r="K38" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
@@ -3808,7 +3822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19">
         <v>68</v>
       </c>
@@ -3832,7 +3846,7 @@
         <v>65</v>
       </c>
       <c r="K39" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
@@ -3846,7 +3860,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="19">
         <v>69</v>
       </c>
@@ -3870,7 +3884,7 @@
         <v>65</v>
       </c>
       <c r="K40" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
@@ -3884,7 +3898,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19">
         <v>70</v>
       </c>
@@ -3908,7 +3922,7 @@
         <v>65</v>
       </c>
       <c r="K41" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
@@ -3922,7 +3936,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="225.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="19">
         <v>71</v>
       </c>
@@ -3945,10 +3959,10 @@
         <v>45104.426342592589</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J42" s="36" t="s">
         <v>38</v>
@@ -3961,13 +3975,13 @@
         <v>38</v>
       </c>
       <c r="N42" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O42" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P42" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q42" s="15"/>
       <c r="R42" s="16"/>
@@ -3976,7 +3990,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="225.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="19">
         <v>72</v>
       </c>
@@ -3999,10 +4013,10 @@
         <v>45104.427581018521</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J43" s="15" t="s">
         <v>38</v>
@@ -4015,13 +4029,13 @@
         <v>38</v>
       </c>
       <c r="N43" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O43" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P43" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q43" s="15"/>
       <c r="R43" s="16"/>
@@ -4030,7 +4044,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="225.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="19">
         <v>73</v>
       </c>
@@ -4053,10 +4067,10 @@
         <v>45104.428587962961</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J44" s="15" t="s">
         <v>38</v>
@@ -4069,13 +4083,13 @@
         <v>38</v>
       </c>
       <c r="N44" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O44" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P44" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q44" s="15"/>
       <c r="R44" s="16"/>
@@ -4084,7 +4098,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
         <v>74</v>
       </c>
@@ -4107,10 +4121,10 @@
         <v>45104.429884259262</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J45" s="15" t="s">
         <v>38</v>
@@ -4123,13 +4137,13 @@
         <v>38</v>
       </c>
       <c r="N45" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="O45" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P45" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q45" s="15"/>
       <c r="R45" s="16"/>
@@ -4138,7 +4152,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="19">
         <v>75</v>
       </c>
@@ -4146,13 +4160,13 @@
         <v>25</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F46" s="13">
         <v>45105</v>
@@ -4161,10 +4175,10 @@
         <v>45105.604085648149</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="J46" s="15" t="s">
         <v>38</v>
@@ -4177,13 +4191,13 @@
         <v>38</v>
       </c>
       <c r="N46" s="15" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="O46" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P46" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q46" s="15"/>
       <c r="R46" s="16"/>
@@ -4192,7 +4206,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <v>76</v>
       </c>
@@ -4200,13 +4214,13 @@
         <v>25</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F47" s="13"/>
       <c r="G47" s="14"/>
@@ -4216,7 +4230,7 @@
         <v>65</v>
       </c>
       <c r="K47" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
@@ -4230,7 +4244,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="19">
         <v>77</v>
       </c>
@@ -4238,13 +4252,13 @@
         <v>25</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F48" s="13"/>
       <c r="G48" s="14"/>
@@ -4254,7 +4268,7 @@
         <v>65</v>
       </c>
       <c r="K48" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
@@ -4268,7 +4282,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="19">
         <v>78</v>
       </c>
@@ -4276,13 +4290,13 @@
         <v>25</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F49" s="13"/>
       <c r="G49" s="14"/>
@@ -4292,7 +4306,7 @@
         <v>65</v>
       </c>
       <c r="K49" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
@@ -4306,7 +4320,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="19">
         <v>79</v>
       </c>
@@ -4314,13 +4328,13 @@
         <v>25</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="14"/>
@@ -4330,7 +4344,7 @@
         <v>65</v>
       </c>
       <c r="K50" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
@@ -4344,7 +4358,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="19">
         <v>80</v>
       </c>
@@ -4352,13 +4366,13 @@
         <v>25</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F51" s="13">
         <v>45105</v>
@@ -4367,10 +4381,10 @@
         <v>45105.675555555557</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J51" s="15" t="s">
         <v>38</v>
@@ -4383,13 +4397,13 @@
         <v>38</v>
       </c>
       <c r="N51" s="15" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="O51" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P51" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q51" s="15"/>
       <c r="R51" s="16"/>
@@ -4398,7 +4412,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="19">
         <v>81</v>
       </c>
@@ -4406,13 +4420,13 @@
         <v>25</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F52" s="13"/>
       <c r="G52" s="14"/>
@@ -4422,7 +4436,7 @@
         <v>65</v>
       </c>
       <c r="K52" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
@@ -4436,7 +4450,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="19">
         <v>82</v>
       </c>
@@ -4444,13 +4458,13 @@
         <v>25</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F53" s="13">
         <v>45105</v>
@@ -4459,10 +4473,10 @@
         <v>45105.691793981481</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="J53" s="15" t="s">
         <v>38</v>
@@ -4475,13 +4489,13 @@
         <v>38</v>
       </c>
       <c r="N53" s="15" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="O53" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P53" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q53" s="15"/>
       <c r="R53" s="16"/>
@@ -4490,7 +4504,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="19">
         <v>83</v>
       </c>
@@ -4498,13 +4512,13 @@
         <v>25</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F54" s="13"/>
       <c r="G54" s="14"/>
@@ -4514,7 +4528,7 @@
         <v>65</v>
       </c>
       <c r="K54" s="15" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
@@ -4528,7 +4542,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="19">
         <v>84</v>
       </c>
@@ -4536,13 +4550,13 @@
         <v>25</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F55" s="13">
         <v>45105</v>
@@ -4551,10 +4565,10 @@
         <v>45105.717881944445</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J55" s="15" t="s">
         <v>38</v>
@@ -4567,13 +4581,13 @@
         <v>38</v>
       </c>
       <c r="N55" s="15" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="O55" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P55" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q55" s="15"/>
       <c r="R55" s="16"/>
@@ -4582,7 +4596,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="19">
         <v>85</v>
       </c>
@@ -4590,13 +4604,13 @@
         <v>25</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F56" s="13"/>
       <c r="G56" s="14"/>
@@ -4606,7 +4620,7 @@
         <v>65</v>
       </c>
       <c r="K56" s="15" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
@@ -4620,7 +4634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="19">
         <v>86</v>
       </c>
@@ -4628,13 +4642,13 @@
         <v>25</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F57" s="13"/>
       <c r="G57" s="14"/>
@@ -4644,7 +4658,7 @@
         <v>65</v>
       </c>
       <c r="K57" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
@@ -4658,7 +4672,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="19">
         <v>87</v>
       </c>
@@ -4666,13 +4680,13 @@
         <v>25</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F58" s="13"/>
       <c r="G58" s="14"/>
@@ -4682,7 +4696,7 @@
         <v>65</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
@@ -4696,7 +4710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="19">
         <v>88</v>
       </c>
@@ -4704,13 +4718,13 @@
         <v>25</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F59" s="13"/>
       <c r="G59" s="14"/>
@@ -4720,7 +4734,7 @@
         <v>65</v>
       </c>
       <c r="K59" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
@@ -4734,7 +4748,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="19">
         <v>89</v>
       </c>
@@ -4742,13 +4756,13 @@
         <v>25</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F60" s="13"/>
       <c r="G60" s="14"/>
@@ -4758,7 +4772,7 @@
         <v>65</v>
       </c>
       <c r="K60" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
@@ -4772,7 +4786,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="19">
         <v>90</v>
       </c>
@@ -4780,13 +4794,13 @@
         <v>25</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D61" s="11" t="s">
+        <v>370</v>
+      </c>
+      <c r="E61" s="12" t="s">
         <v>372</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>374</v>
       </c>
       <c r="F61" s="13"/>
       <c r="G61" s="14"/>
@@ -4796,7 +4810,7 @@
         <v>65</v>
       </c>
       <c r="K61" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L61" s="15"/>
       <c r="M61" s="15"/>
@@ -4810,7 +4824,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="19">
         <v>91</v>
       </c>
@@ -4818,13 +4832,13 @@
         <v>25</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D62" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="E62" s="12" t="s">
         <v>373</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>375</v>
       </c>
       <c r="F62" s="13"/>
       <c r="G62" s="14"/>
@@ -4834,7 +4848,7 @@
         <v>65</v>
       </c>
       <c r="K62" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L62" s="15"/>
       <c r="M62" s="15"/>
@@ -4848,7 +4862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="19">
         <v>92</v>
       </c>
@@ -4856,13 +4870,13 @@
         <v>25</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F63" s="13"/>
       <c r="G63" s="14"/>
@@ -4872,7 +4886,7 @@
         <v>65</v>
       </c>
       <c r="K63" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L63" s="15"/>
       <c r="M63" s="15"/>
@@ -4886,7 +4900,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="19">
         <v>93</v>
       </c>
@@ -4894,13 +4908,13 @@
         <v>25</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F64" s="13"/>
       <c r="G64" s="14"/>
@@ -4910,7 +4924,7 @@
         <v>65</v>
       </c>
       <c r="K64" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L64" s="15"/>
       <c r="M64" s="15"/>
@@ -4924,7 +4938,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="19">
         <v>122</v>
       </c>
@@ -4932,13 +4946,13 @@
         <v>25</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D65" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E65" s="12" t="s">
         <v>100</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>101</v>
       </c>
       <c r="F65" s="13"/>
       <c r="G65" s="14"/>
@@ -4948,7 +4962,7 @@
         <v>65</v>
       </c>
       <c r="K65" s="15" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="L65" s="15"/>
       <c r="M65" s="15"/>
@@ -4962,7 +4976,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="19">
         <v>123</v>
       </c>
@@ -4970,13 +4984,13 @@
         <v>25</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D66" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E66" s="12" t="s">
         <v>102</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>103</v>
       </c>
       <c r="F66" s="13"/>
       <c r="G66" s="14"/>
@@ -4986,7 +5000,7 @@
         <v>65</v>
       </c>
       <c r="K66" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L66" s="15"/>
       <c r="M66" s="15"/>
@@ -5000,7 +5014,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="19">
         <v>124</v>
       </c>
@@ -5008,13 +5022,13 @@
         <v>25</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D67" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E67" s="12" t="s">
         <v>104</v>
-      </c>
-      <c r="E67" s="12" t="s">
-        <v>105</v>
       </c>
       <c r="F67" s="13">
         <v>45104</v>
@@ -5023,10 +5037,10 @@
         <v>45104.434178240743</v>
       </c>
       <c r="H67" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I67" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J67" s="15" t="s">
         <v>38</v>
@@ -5038,13 +5052,13 @@
         <v>38</v>
       </c>
       <c r="N67" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O67" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P67" s="15" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="Q67" s="15"/>
       <c r="R67" s="16"/>
@@ -5053,7 +5067,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="19">
         <v>125</v>
       </c>
@@ -5061,13 +5075,13 @@
         <v>25</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D68" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E68" s="12" t="s">
         <v>106</v>
-      </c>
-      <c r="E68" s="12" t="s">
-        <v>107</v>
       </c>
       <c r="F68" s="13"/>
       <c r="G68" s="14"/>
@@ -5077,7 +5091,7 @@
         <v>65</v>
       </c>
       <c r="K68" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L68" s="15"/>
       <c r="M68" s="15"/>
@@ -5091,7 +5105,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="19">
         <v>126</v>
       </c>
@@ -5099,13 +5113,13 @@
         <v>25</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D69" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E69" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>109</v>
       </c>
       <c r="F69" s="13"/>
       <c r="G69" s="14"/>
@@ -5115,7 +5129,7 @@
         <v>65</v>
       </c>
       <c r="K69" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L69" s="15"/>
       <c r="M69" s="15"/>
@@ -5129,7 +5143,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="19">
         <v>127</v>
       </c>
@@ -5137,13 +5151,13 @@
         <v>25</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D70" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E70" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="E70" s="12" t="s">
-        <v>111</v>
       </c>
       <c r="F70" s="13"/>
       <c r="G70" s="14"/>
@@ -5153,7 +5167,7 @@
         <v>65</v>
       </c>
       <c r="K70" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L70" s="15"/>
       <c r="M70" s="15"/>
@@ -5167,7 +5181,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="19">
         <v>128</v>
       </c>
@@ -5175,13 +5189,13 @@
         <v>25</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D71" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E71" s="12" t="s">
         <v>112</v>
-      </c>
-      <c r="E71" s="12" t="s">
-        <v>113</v>
       </c>
       <c r="F71" s="13"/>
       <c r="G71" s="14"/>
@@ -5191,7 +5205,7 @@
         <v>65</v>
       </c>
       <c r="K71" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L71" s="15"/>
       <c r="M71" s="15"/>
@@ -5205,7 +5219,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="19">
         <v>129</v>
       </c>
@@ -5213,13 +5227,13 @@
         <v>25</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F72" s="13">
         <v>45104</v>
@@ -5228,10 +5242,10 @@
         <v>45104.435486111113</v>
       </c>
       <c r="H72" s="37" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="I72" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J72" s="15" t="s">
         <v>38</v>
@@ -5244,13 +5258,13 @@
         <v>38</v>
       </c>
       <c r="N72" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="O72" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P72" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q72" s="15"/>
       <c r="R72" s="16"/>
@@ -5259,7 +5273,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="19">
         <v>130</v>
       </c>
@@ -5267,13 +5281,13 @@
         <v>25</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D73" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E73" s="12" t="s">
         <v>116</v>
-      </c>
-      <c r="E73" s="12" t="s">
-        <v>117</v>
       </c>
       <c r="F73" s="13">
         <v>45104</v>
@@ -5282,10 +5296,10 @@
         <v>45104.436909722222</v>
       </c>
       <c r="H73" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I73" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J73" s="15" t="s">
         <v>38</v>
@@ -5298,13 +5312,13 @@
         <v>38</v>
       </c>
       <c r="N73" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="O73" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P73" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q73" s="15"/>
       <c r="R73" s="16"/>
@@ -5313,7 +5327,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="19">
         <v>131</v>
       </c>
@@ -5321,13 +5335,13 @@
         <v>25</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D74" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E74" s="12" t="s">
         <v>118</v>
-      </c>
-      <c r="E74" s="12" t="s">
-        <v>119</v>
       </c>
       <c r="F74" s="13">
         <v>45104</v>
@@ -5336,10 +5350,10 @@
         <v>45104.438668981478</v>
       </c>
       <c r="H74" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I74" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J74" s="15" t="s">
         <v>38</v>
@@ -5352,13 +5366,13 @@
         <v>38</v>
       </c>
       <c r="N74" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="O74" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P74" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q74" s="15"/>
       <c r="R74" s="16"/>
@@ -5367,7 +5381,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="19">
         <v>132</v>
       </c>
@@ -5375,13 +5389,13 @@
         <v>25</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F75" s="13">
         <v>45104</v>
@@ -5390,10 +5404,10 @@
         <v>45104.439479166664</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I75" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="J75" s="15" t="s">
         <v>38</v>
@@ -5406,13 +5420,13 @@
         <v>38</v>
       </c>
       <c r="N75" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O75" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P75" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q75" s="15"/>
       <c r="R75" s="16"/>
@@ -5421,7 +5435,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="19">
         <v>133</v>
       </c>
@@ -5429,13 +5443,13 @@
         <v>25</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F76" s="13"/>
       <c r="G76" s="14"/>
@@ -5445,7 +5459,7 @@
         <v>65</v>
       </c>
       <c r="K76" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L76" s="15"/>
       <c r="M76" s="15"/>
@@ -5459,7 +5473,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="19">
         <v>134</v>
       </c>
@@ -5467,13 +5481,13 @@
         <v>25</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F77" s="13"/>
       <c r="G77" s="14"/>
@@ -5483,7 +5497,7 @@
         <v>65</v>
       </c>
       <c r="K77" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L77" s="15"/>
       <c r="M77" s="15"/>
@@ -5497,7 +5511,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="19">
         <v>135</v>
       </c>
@@ -5505,13 +5519,13 @@
         <v>25</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F78" s="13">
         <v>45104</v>
@@ -5520,10 +5534,10 @@
         <v>45104.442962962959</v>
       </c>
       <c r="H78" s="14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I78" s="14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J78" s="15" t="s">
         <v>38</v>
@@ -5536,13 +5550,13 @@
         <v>38</v>
       </c>
       <c r="N78" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O78" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P78" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q78" s="15"/>
       <c r="R78" s="16"/>
@@ -5551,7 +5565,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="19">
         <v>136</v>
       </c>
@@ -5559,13 +5573,13 @@
         <v>25</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E79" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F79" s="13"/>
       <c r="G79" s="14"/>
@@ -5575,7 +5589,7 @@
         <v>65</v>
       </c>
       <c r="K79" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M79" s="15"/>
       <c r="N79" s="15"/>
@@ -5588,7 +5602,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="19">
         <v>137</v>
       </c>
@@ -5596,13 +5610,13 @@
         <v>25</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E80" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F80" s="13">
         <v>45104</v>
@@ -5611,10 +5625,10 @@
         <v>45104.443761574075</v>
       </c>
       <c r="H80" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I80" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J80" s="15" t="s">
         <v>38</v>
@@ -5627,13 +5641,13 @@
         <v>38</v>
       </c>
       <c r="N80" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O80" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P80" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q80" s="15"/>
       <c r="R80" s="16"/>
@@ -5642,7 +5656,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="19">
         <v>138</v>
       </c>
@@ -5650,13 +5664,13 @@
         <v>25</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F81" s="13">
         <v>45104</v>
@@ -5665,10 +5679,10 @@
         <v>45104.444768518515</v>
       </c>
       <c r="H81" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I81" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J81" s="15" t="s">
         <v>38</v>
@@ -5681,13 +5695,13 @@
         <v>38</v>
       </c>
       <c r="N81" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="O81" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P81" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q81" s="15"/>
       <c r="R81" s="16"/>
@@ -5696,7 +5710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="19">
         <v>139</v>
       </c>
@@ -5704,13 +5718,13 @@
         <v>25</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F82" s="13"/>
       <c r="G82" s="14"/>
@@ -5720,7 +5734,7 @@
         <v>65</v>
       </c>
       <c r="K82" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L82" s="15"/>
       <c r="M82" s="15"/>
@@ -5734,7 +5748,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="19">
         <v>140</v>
       </c>
@@ -5742,13 +5756,13 @@
         <v>25</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E83" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F83" s="13"/>
       <c r="G83" s="14"/>
@@ -5758,7 +5772,7 @@
         <v>65</v>
       </c>
       <c r="K83" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L83" s="15"/>
       <c r="M83" s="15"/>
@@ -5772,7 +5786,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="19">
         <v>141</v>
       </c>
@@ -5780,13 +5794,13 @@
         <v>25</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F84" s="13">
         <v>45104</v>
@@ -5795,10 +5809,10 @@
         <v>45104.445601851854</v>
       </c>
       <c r="H84" s="14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I84" s="38" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J84" s="15" t="s">
         <v>38</v>
@@ -5811,13 +5825,13 @@
         <v>38</v>
       </c>
       <c r="N84" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="O84" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P84" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q84" s="15"/>
       <c r="R84" s="16"/>
@@ -5826,7 +5840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="19">
         <v>142</v>
       </c>
@@ -5834,13 +5848,13 @@
         <v>25</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F85" s="13">
         <v>45104</v>
@@ -5849,10 +5863,10 @@
         <v>45104.446585648147</v>
       </c>
       <c r="H85" s="14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I85" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J85" s="15" t="s">
         <v>38</v>
@@ -5865,13 +5879,13 @@
         <v>38</v>
       </c>
       <c r="N85" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="O85" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P85" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q85" s="15"/>
       <c r="R85" s="16"/>
@@ -5880,7 +5894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="19">
         <v>143</v>
       </c>
@@ -5888,13 +5902,13 @@
         <v>25</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E86" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F86" s="13">
         <v>45104</v>
@@ -5903,10 +5917,10 @@
         <v>45104.447384259256</v>
       </c>
       <c r="H86" s="14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I86" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J86" s="15" t="s">
         <v>38</v>
@@ -5919,13 +5933,13 @@
         <v>38</v>
       </c>
       <c r="N86" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="O86" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P86" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q86" s="15"/>
       <c r="R86" s="16"/>
@@ -5934,7 +5948,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="19">
         <v>144</v>
       </c>
@@ -5942,13 +5956,13 @@
         <v>25</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E87" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F87" s="13">
         <v>45104</v>
@@ -5957,10 +5971,10 @@
         <v>45104.449189814812</v>
       </c>
       <c r="H87" s="14" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I87" s="14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J87" s="15" t="s">
         <v>38</v>
@@ -5973,13 +5987,13 @@
         <v>38</v>
       </c>
       <c r="N87" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="O87" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P87" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q87" s="15"/>
       <c r="R87" s="16"/>
@@ -5988,7 +6002,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="19">
         <v>145</v>
       </c>
@@ -5996,13 +6010,13 @@
         <v>25</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E88" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F88" s="13"/>
       <c r="G88" s="14"/>
@@ -6012,7 +6026,7 @@
         <v>65</v>
       </c>
       <c r="K88" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L88" s="15"/>
       <c r="M88" s="15"/>
@@ -6026,7 +6040,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="98.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" ht="98.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="19">
         <v>146</v>
       </c>
@@ -6034,13 +6048,13 @@
         <v>25</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E89" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F89" s="13">
         <v>45104</v>
@@ -6049,10 +6063,10 @@
         <v>45104.450011574074</v>
       </c>
       <c r="H89" s="14" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I89" s="14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J89" s="15" t="s">
         <v>38</v>
@@ -6065,13 +6079,13 @@
         <v>38</v>
       </c>
       <c r="N89" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="O89" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P89" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q89" s="15"/>
       <c r="R89" s="16"/>
@@ -6080,7 +6094,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="19">
         <v>147</v>
       </c>
@@ -6088,13 +6102,13 @@
         <v>25</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E90" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F90" s="13">
         <v>45104</v>
@@ -6103,10 +6117,10 @@
         <v>45104.450856481482</v>
       </c>
       <c r="H90" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I90" s="14" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J90" s="15" t="s">
         <v>38</v>
@@ -6128,7 +6142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="19">
         <v>148</v>
       </c>
@@ -6136,13 +6150,13 @@
         <v>25</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E91" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F91" s="13"/>
       <c r="G91" s="14"/>
@@ -6152,7 +6166,7 @@
         <v>65</v>
       </c>
       <c r="K91" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L91" s="15"/>
       <c r="M91" s="15"/>
@@ -6166,7 +6180,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="19">
         <v>149</v>
       </c>
@@ -6174,13 +6188,13 @@
         <v>25</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E92" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F92" s="13"/>
       <c r="G92" s="14"/>
@@ -6190,7 +6204,7 @@
         <v>65</v>
       </c>
       <c r="K92" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L92" s="15"/>
       <c r="M92" s="15"/>
@@ -6204,7 +6218,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="19">
         <v>150</v>
       </c>
@@ -6212,13 +6226,13 @@
         <v>25</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F93" s="13"/>
       <c r="G93" s="14"/>
@@ -6228,7 +6242,7 @@
         <v>65</v>
       </c>
       <c r="K93" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L93" s="15"/>
       <c r="M93" s="15"/>
@@ -6242,7 +6256,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="19">
         <v>151</v>
       </c>
@@ -6250,13 +6264,13 @@
         <v>25</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E94" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F94" s="13">
         <v>45104</v>
@@ -6265,10 +6279,10 @@
         <v>45104.451840277776</v>
       </c>
       <c r="H94" s="14" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I94" s="14" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J94" s="15" t="s">
         <v>38</v>
@@ -6281,13 +6295,13 @@
         <v>38</v>
       </c>
       <c r="N94" s="15" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O94" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P94" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q94" s="15"/>
       <c r="R94" s="16"/>
@@ -6296,7 +6310,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="19">
         <v>152</v>
       </c>
@@ -6304,13 +6318,13 @@
         <v>25</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F95" s="13"/>
       <c r="G95" s="14"/>
@@ -6320,7 +6334,7 @@
         <v>65</v>
       </c>
       <c r="K95" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L95" s="15"/>
       <c r="M95" s="15"/>
@@ -6334,7 +6348,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="19">
         <v>153</v>
       </c>
@@ -6342,13 +6356,13 @@
         <v>25</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F96" s="13">
         <v>45111</v>
@@ -6357,10 +6371,10 @@
         <v>45111.63380787037</v>
       </c>
       <c r="H96" s="14" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I96" s="14" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J96" s="15" t="s">
         <v>38</v>
@@ -6373,13 +6387,13 @@
         <v>38</v>
       </c>
       <c r="N96" s="15" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="O96" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P96" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q96" s="15"/>
       <c r="R96" s="16"/>
@@ -6388,7 +6402,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="19">
         <v>154</v>
       </c>
@@ -6396,13 +6410,13 @@
         <v>25</v>
       </c>
       <c r="C97" s="42" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F97" s="13"/>
       <c r="G97" s="14"/>
@@ -6412,7 +6426,7 @@
         <v>65</v>
       </c>
       <c r="K97" s="15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="L97" s="15"/>
       <c r="M97" s="15"/>
@@ -6426,7 +6440,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="19">
         <v>155</v>
       </c>
@@ -6434,13 +6448,13 @@
         <v>25</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F98" s="13"/>
       <c r="G98" s="14"/>
@@ -6450,7 +6464,7 @@
         <v>65</v>
       </c>
       <c r="K98" s="15" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="L98" s="15"/>
       <c r="M98" s="15"/>
@@ -6464,7 +6478,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="19">
         <v>156</v>
       </c>
@@ -6472,13 +6486,13 @@
         <v>25</v>
       </c>
       <c r="C99" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D99" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E99" s="12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F99" s="13"/>
       <c r="G99" s="14"/>
@@ -6488,7 +6502,7 @@
         <v>65</v>
       </c>
       <c r="K99" s="15" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L99" s="15"/>
       <c r="M99" s="15"/>
@@ -6502,7 +6516,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="19">
         <v>157</v>
       </c>
@@ -6510,13 +6524,13 @@
         <v>25</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E100" s="12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F100" s="13"/>
       <c r="G100" s="14"/>
@@ -6526,7 +6540,7 @@
         <v>65</v>
       </c>
       <c r="K100" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L100" s="15"/>
       <c r="M100" s="15"/>
@@ -6540,7 +6554,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="19">
         <v>158</v>
       </c>
@@ -6548,13 +6562,13 @@
         <v>25</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E101" s="12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F101" s="13">
         <v>45104</v>
@@ -6563,10 +6577,10 @@
         <v>45104.454525462963</v>
       </c>
       <c r="H101" s="14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I101" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J101" s="15" t="s">
         <v>38</v>
@@ -6579,13 +6593,13 @@
         <v>38</v>
       </c>
       <c r="N101" s="15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="O101" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P101" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q101" s="15"/>
       <c r="R101" s="16"/>
@@ -6594,7 +6608,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="19">
         <v>159</v>
       </c>
@@ -6602,13 +6616,13 @@
         <v>25</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E102" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F102" s="13">
         <v>45104</v>
@@ -6617,10 +6631,10 @@
         <v>45104.455439814818</v>
       </c>
       <c r="H102" s="14" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I102" s="14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J102" s="15" t="s">
         <v>38</v>
@@ -6633,13 +6647,13 @@
         <v>38</v>
       </c>
       <c r="N102" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="O102" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P102" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q102" s="15"/>
       <c r="R102" s="16"/>
@@ -6648,7 +6662,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="19">
         <v>160</v>
       </c>
@@ -6656,13 +6670,13 @@
         <v>25</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F103" s="13">
         <v>45104</v>
@@ -6671,10 +6685,10 @@
         <v>45104.456284722219</v>
       </c>
       <c r="H103" s="14" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I103" s="14" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J103" s="15" t="s">
         <v>38</v>
@@ -6687,13 +6701,13 @@
         <v>38</v>
       </c>
       <c r="N103" s="15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O103" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P103" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q103" s="15"/>
       <c r="R103" s="16"/>
@@ -6702,7 +6716,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="19">
         <v>161</v>
       </c>
@@ -6710,13 +6724,13 @@
         <v>25</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F104" s="13">
         <v>45104</v>
@@ -6725,10 +6739,10 @@
         <v>45104.457465277781</v>
       </c>
       <c r="H104" s="14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I104" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J104" s="15" t="s">
         <v>38</v>
@@ -6741,13 +6755,13 @@
         <v>38</v>
       </c>
       <c r="N104" s="15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O104" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P104" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q104" s="15"/>
       <c r="R104" s="16"/>
@@ -6756,7 +6770,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:20" s="33" customFormat="1" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:20" s="33" customFormat="1" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="23">
         <v>162</v>
       </c>
@@ -6764,13 +6778,13 @@
         <v>25</v>
       </c>
       <c r="C105" s="24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D105" s="24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E105" s="25" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F105" s="26">
         <v>45104</v>
@@ -6779,10 +6793,10 @@
         <v>45104.772928240738</v>
       </c>
       <c r="H105" s="27" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I105" s="27" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="J105" s="29" t="s">
         <v>38</v>
@@ -6795,13 +6809,13 @@
         <v>38</v>
       </c>
       <c r="N105" s="29" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="O105" s="29" t="s">
         <v>38</v>
       </c>
       <c r="P105" s="29" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q105" s="29"/>
       <c r="R105" s="30"/>
@@ -6810,7 +6824,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="19">
         <v>163</v>
       </c>
@@ -6818,13 +6832,13 @@
         <v>25</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D106" s="11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E106" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F106" s="13"/>
       <c r="G106" s="14"/>
@@ -6834,7 +6848,7 @@
         <v>65</v>
       </c>
       <c r="K106" s="15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L106" s="15"/>
       <c r="M106" s="15"/>
@@ -6848,7 +6862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="19">
         <v>164</v>
       </c>
@@ -6856,13 +6870,13 @@
         <v>25</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D107" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F107" s="13">
         <v>45104</v>
@@ -6871,10 +6885,10 @@
         <v>45104.464988425927</v>
       </c>
       <c r="H107" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I107" s="14" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J107" s="15" t="s">
         <v>38</v>
@@ -6887,13 +6901,13 @@
         <v>38</v>
       </c>
       <c r="N107" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="O107" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P107" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q107" s="15"/>
       <c r="R107" s="16"/>
@@ -6902,7 +6916,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="98.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:20" ht="98.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="19">
         <v>165</v>
       </c>
@@ -6910,13 +6924,13 @@
         <v>25</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E108" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F108" s="13">
         <v>45104</v>
@@ -6925,10 +6939,10 @@
         <v>45104.773680555554</v>
       </c>
       <c r="H108" s="14" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I108" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="J108" s="15" t="s">
         <v>38</v>
@@ -6941,13 +6955,13 @@
         <v>38</v>
       </c>
       <c r="N108" s="15" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O108" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P108" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q108" s="15"/>
       <c r="R108" s="16"/>
@@ -6956,7 +6970,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="19">
         <v>166</v>
       </c>
@@ -6964,13 +6978,13 @@
         <v>25</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E109" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F109" s="13">
         <v>45104</v>
@@ -6979,10 +6993,10 @@
         <v>45104.774641203701</v>
       </c>
       <c r="H109" s="14" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I109" s="14" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J109" s="15" t="s">
         <v>38</v>
@@ -6995,13 +7009,13 @@
         <v>38</v>
       </c>
       <c r="N109" s="15" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="O109" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P109" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q109" s="15"/>
       <c r="R109" s="16"/>
@@ -7010,7 +7024,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="19">
         <v>167</v>
       </c>
@@ -7018,13 +7032,13 @@
         <v>25</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E110" s="12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F110" s="13">
         <v>45104</v>
@@ -7033,10 +7047,10 @@
         <v>45104.775740740741</v>
       </c>
       <c r="H110" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I110" s="14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J110" s="15" t="s">
         <v>38</v>
@@ -7049,13 +7063,13 @@
         <v>38</v>
       </c>
       <c r="N110" s="15" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="O110" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P110" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q110" s="15"/>
       <c r="R110" s="16"/>
@@ -7064,7 +7078,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="19">
         <v>168</v>
       </c>
@@ -7072,13 +7086,13 @@
         <v>25</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E111" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F111" s="13"/>
       <c r="G111" s="14"/>
@@ -7088,7 +7102,7 @@
         <v>65</v>
       </c>
       <c r="K111" s="15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L111" s="15"/>
       <c r="M111" s="15"/>
@@ -7102,7 +7116,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="19">
         <v>169</v>
       </c>
@@ -7110,13 +7124,13 @@
         <v>25</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D112" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E112" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F112" s="13">
         <v>45104</v>
@@ -7125,10 +7139,10 @@
         <v>45104.776620370372</v>
       </c>
       <c r="H112" s="14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I112" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J112" s="15" t="s">
         <v>38</v>
@@ -7141,13 +7155,13 @@
         <v>38</v>
       </c>
       <c r="N112" s="15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O112" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P112" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q112" s="15"/>
       <c r="R112" s="16"/>
@@ -7156,7 +7170,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="1:21" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:21" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="19">
         <v>369</v>
       </c>
@@ -7167,7 +7181,7 @@
         <v>24</v>
       </c>
       <c r="D113" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E113" s="12"/>
       <c r="F113" s="13">
@@ -7177,10 +7191,10 @@
         <v>45104.777511574073</v>
       </c>
       <c r="H113" s="14" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I113" s="14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="J113" s="15" t="s">
         <v>38</v>
@@ -7202,7 +7216,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="114" spans="1:21" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:21" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="19">
         <v>370</v>
       </c>
@@ -7210,10 +7224,10 @@
         <v>25</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D114" s="11" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E114" s="12"/>
       <c r="F114" s="13">
@@ -7223,10 +7237,10 @@
         <v>45105.704733796294</v>
       </c>
       <c r="H114" s="14" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I114" s="14" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="J114" s="15" t="s">
         <v>38</v>
@@ -7239,7 +7253,7 @@
         <v>38</v>
       </c>
       <c r="P114" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q114" s="15"/>
       <c r="R114" s="16"/>
@@ -7248,7 +7262,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="115" spans="1:21" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:21" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="19">
         <v>373</v>
       </c>
@@ -7256,10 +7270,10 @@
         <v>25</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D115" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E115" s="12"/>
       <c r="F115" s="13">
@@ -7269,10 +7283,10 @@
         <v>45104.778263888889</v>
       </c>
       <c r="H115" s="14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I115" s="14" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="J115" s="15" t="s">
         <v>38</v>
@@ -7294,7 +7308,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="116" spans="1:21" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:21" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="19">
         <v>374</v>
       </c>
@@ -7302,10 +7316,10 @@
         <v>25</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D116" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E116" s="12"/>
       <c r="F116" s="13">
@@ -7315,10 +7329,10 @@
         <v>45104.779027777775</v>
       </c>
       <c r="H116" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="I116" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J116" s="15" t="s">
         <v>38</v>
@@ -16940,7 +16954,16 @@
       <c r="T736" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T116" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="A9:T116" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="VALIDAZIONE_LDO_TIMEOUT"/>
+        <filter val="VALIDAZIONE_RAD_TIMEOUT"/>
+        <filter val="VALIDAZIONE_RSA_TIMEOUT"/>
+        <filter val="VALIDAZIONE_VPS_TIMEOUT"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>

</xml_diff>

<commit_message>
MODIFICHE A SEGUITO DI SEGNALAZIONE
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111NBSSRLXXXXX/NBS/networksanitario/v.4.10.106/report-checklist.xlsx
+++ b/GATEWAY/S1#111NBSSRLXXXXX/NBS/networksanitario/v.4.10.106/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.damiani\Desktop\it-fse-accreditamento\GATEWAY\S1#111NBSSRLXXXXX\NBS\networksanitario\v.4.10.106\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E1DA6B-293F-4058-92FE-2E56117CC7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7785EA-5565-45D7-86BB-ACAB56BBB8B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="345" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
@@ -390,9 +390,6 @@
     <t>subject_application_version:v.4.10.106</t>
   </si>
   <si>
-    <t>Viene segnalato un errore di connessione al gateway e si chiede di segnalare il problema all'amministratore di sistema</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT7_KO </t>
   </si>
   <si>
@@ -1499,13 +1496,17 @@
     <t>ae6aa4deccc52eba</t>
   </si>
   <si>
-    <t>In caso di errore il processo applicativo prosegue ed il documento viene firmato. Eventuali verifiche, correzioni dei dati e re-invii vengono concordati/definiti con le singole aziende.
-Viene messo a disposizione dell'azienda una modalità di verifica dei documenti che hanno avuto errori di validazione da parte del gateway per poterli individuare e procedere alla correzione, firma e re-invio.?</t>
-  </si>
-  <si>
     <t>Attenzione!
 Il servizio di validazione ha impiegato troppo tempo a rispondere. 
 Procedere alla firma?</t>
+  </si>
+  <si>
+    <t>In caso di errore il processo applicativo prosegue ed il documento viene firmato. Eventuali verifiche, correzioni dei dati e re-invii vengono concordati/definiti con le singole aziende.
+Viene messo a disposizione dell'azienda una modalità di verifica dei documenti che hanno avuto errori di validazione da parte del gateway per poterli individuareTali documenti verranno inseriti in una coda e reinviati in maniera automatica al gatawy</t>
+  </si>
+  <si>
+    <t>IIn caso di errore il processo applicativo prosegue ed il documento viene firmato. Eventuali verifiche, correzioni dei dati e re-invii vengono concordati/definiti con le singole aziende.
+Viene messo a disposizione dell'azienda una modalità di verifica dei documenti che hanno avuto errori di validazione da parte del gateway per poterli individuareTali documenti verranno inseriti in una coda e reinviati in maniera automatica al gatawy</t>
   </si>
 </sst>
 </file>
@@ -2232,14 +2233,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:U736"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2493,7 +2493,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>6</v>
       </c>
@@ -2516,10 +2516,10 @@
         <v>45104.40084490741</v>
       </c>
       <c r="H10" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="I10" s="14" t="s">
         <v>253</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>254</v>
       </c>
       <c r="J10" s="15" t="s">
         <v>38</v>
@@ -2541,7 +2541,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>7</v>
       </c>
@@ -2564,10 +2564,10 @@
         <v>45104.402025462965</v>
       </c>
       <c r="H11" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="I11" s="14" t="s">
         <v>255</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>256</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>38</v>
@@ -2589,7 +2589,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>8</v>
       </c>
@@ -2612,10 +2612,10 @@
         <v>45104.403078703705</v>
       </c>
       <c r="H12" s="37" t="s">
+        <v>256</v>
+      </c>
+      <c r="I12" s="14" t="s">
         <v>257</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>258</v>
       </c>
       <c r="J12" s="20" t="s">
         <v>38</v>
@@ -2637,7 +2637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>9</v>
       </c>
@@ -2661,12 +2661,12 @@
         <v>65</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
       <c r="N13" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
@@ -2677,7 +2677,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="76.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>11</v>
       </c>
@@ -2685,13 +2685,13 @@
         <v>25</v>
       </c>
       <c r="C14" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="E14" s="34" t="s">
         <v>328</v>
-      </c>
-      <c r="E14" s="34" t="s">
-        <v>329</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="14"/>
@@ -2701,7 +2701,7 @@
         <v>65</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
@@ -2715,7 +2715,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="76.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>12</v>
       </c>
@@ -2723,13 +2723,13 @@
         <v>25</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D15" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="E15" s="34" t="s">
         <v>330</v>
-      </c>
-      <c r="E15" s="34" t="s">
-        <v>331</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="14"/>
@@ -2739,7 +2739,7 @@
         <v>65</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
@@ -2753,7 +2753,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="76.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>13</v>
       </c>
@@ -2761,13 +2761,13 @@
         <v>25</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="14"/>
@@ -2777,7 +2777,7 @@
         <v>65</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
@@ -2791,7 +2791,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="76.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>14</v>
       </c>
@@ -2799,13 +2799,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="14"/>
@@ -2815,7 +2815,7 @@
         <v>65</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
@@ -2829,7 +2829,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="105" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>24</v>
       </c>
@@ -2837,13 +2837,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="E18" s="34" t="s">
         <v>87</v>
-      </c>
-      <c r="E18" s="34" t="s">
-        <v>88</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="14"/>
@@ -2853,7 +2853,7 @@
         <v>65</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
@@ -2867,7 +2867,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="105" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>25</v>
       </c>
@@ -2875,13 +2875,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D19" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="34" t="s">
         <v>89</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>90</v>
       </c>
       <c r="F19" s="13"/>
       <c r="G19" s="14"/>
@@ -2891,7 +2891,7 @@
         <v>65</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
@@ -2905,7 +2905,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="105" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <v>26</v>
       </c>
@@ -2913,13 +2913,13 @@
         <v>25</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="34" t="s">
         <v>91</v>
-      </c>
-      <c r="E20" s="34" t="s">
-        <v>92</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="14"/>
@@ -2929,7 +2929,7 @@
         <v>65</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
@@ -2943,7 +2943,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="105" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19">
         <v>27</v>
       </c>
@@ -2951,13 +2951,13 @@
         <v>25</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D21" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="34" t="s">
         <v>93</v>
-      </c>
-      <c r="E21" s="34" t="s">
-        <v>94</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="14"/>
@@ -2967,7 +2967,7 @@
         <v>65</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
@@ -2981,7 +2981,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="225.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
         <v>29</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>45104.406759259262</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I22" s="14" t="s">
         <v>66</v>
@@ -3020,13 +3020,13 @@
         <v>38</v>
       </c>
       <c r="N22" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O22" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P22" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q22" s="15"/>
       <c r="R22" s="16"/>
@@ -3035,7 +3035,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="117.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="117.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>31</v>
       </c>
@@ -3043,13 +3043,13 @@
         <v>25</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D23" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>336</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>337</v>
       </c>
       <c r="F23" s="13">
         <v>45105</v>
@@ -3058,7 +3058,7 @@
         <v>45105.520231481481</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I23" s="14" t="s">
         <v>66</v>
@@ -3074,13 +3074,13 @@
         <v>38</v>
       </c>
       <c r="N23" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O23" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P23" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q23" s="15"/>
       <c r="R23" s="16"/>
@@ -3089,7 +3089,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="156" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="156" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>32</v>
       </c>
@@ -3097,13 +3097,13 @@
         <v>25</v>
       </c>
       <c r="C24" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D24" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="D24" s="35" t="s">
+      <c r="E24" s="12" t="s">
         <v>173</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>174</v>
       </c>
       <c r="F24" s="13">
         <v>45104</v>
@@ -3112,7 +3112,7 @@
         <v>45104.407858796294</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I24" s="14" t="s">
         <v>66</v>
@@ -3128,13 +3128,13 @@
         <v>38</v>
       </c>
       <c r="N24" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O24" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P24" s="15" t="s">
-        <v>73</v>
+        <v>395</v>
       </c>
       <c r="Q24" s="15"/>
       <c r="R24" s="16"/>
@@ -3143,7 +3143,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="150" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>35</v>
       </c>
@@ -3151,13 +3151,13 @@
         <v>25</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F25" s="13">
         <v>45104</v>
@@ -3166,7 +3166,7 @@
         <v>45104.410115740742</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I25" s="14" t="s">
         <v>66</v>
@@ -3182,13 +3182,13 @@
         <v>38</v>
       </c>
       <c r="N25" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O25" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P25" s="15" t="s">
-        <v>73</v>
+        <v>395</v>
       </c>
       <c r="Q25" s="15"/>
       <c r="R25" s="16"/>
@@ -3197,7 +3197,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>37</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>45104.412164351852</v>
       </c>
       <c r="H26" s="37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I26" s="14" t="s">
         <v>66</v>
@@ -3242,7 +3242,7 @@
         <v>38</v>
       </c>
       <c r="P26" s="15" t="s">
-        <v>73</v>
+        <v>395</v>
       </c>
       <c r="Q26" s="15"/>
       <c r="R26" s="16"/>
@@ -3253,7 +3253,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="136.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>39</v>
       </c>
@@ -3261,13 +3261,13 @@
         <v>25</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D27" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="E27" s="12" t="s">
         <v>338</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>339</v>
       </c>
       <c r="F27" s="13">
         <v>45105</v>
@@ -3276,7 +3276,7 @@
         <v>45105.52375</v>
       </c>
       <c r="H27" s="37" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I27" s="14" t="s">
         <v>66</v>
@@ -3298,7 +3298,7 @@
         <v>38</v>
       </c>
       <c r="P27" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q27" s="15"/>
       <c r="R27" s="16"/>
@@ -3307,7 +3307,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="110.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>40</v>
       </c>
@@ -3315,13 +3315,13 @@
         <v>25</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F28" s="13">
         <v>45104</v>
@@ -3330,7 +3330,7 @@
         <v>45104.412905092591</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I28" s="14" t="s">
         <v>66</v>
@@ -3346,13 +3346,13 @@
         <v>38</v>
       </c>
       <c r="N28" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O28" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P28" s="15" t="s">
-        <v>73</v>
+        <v>395</v>
       </c>
       <c r="Q28" s="15"/>
       <c r="R28" s="16"/>
@@ -3361,7 +3361,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="87.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
         <v>43</v>
       </c>
@@ -3369,13 +3369,13 @@
         <v>25</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F29" s="13">
         <v>45104</v>
@@ -3384,7 +3384,7 @@
         <v>45104.413842592592</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I29" s="14" t="s">
         <v>66</v>
@@ -3406,7 +3406,7 @@
         <v>38</v>
       </c>
       <c r="P29" s="15" t="s">
-        <v>73</v>
+        <v>395</v>
       </c>
       <c r="Q29" s="15"/>
       <c r="R29" s="16"/>
@@ -3417,7 +3417,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="255.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19">
         <v>45</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>39</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F30" s="13">
         <v>45104</v>
@@ -3452,10 +3452,10 @@
         <v>38</v>
       </c>
       <c r="N30" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="O30" s="15" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="P30" s="15" t="s">
         <v>404</v>
@@ -3475,13 +3475,13 @@
         <v>25</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F31" s="13">
         <v>45105</v>
@@ -3502,10 +3502,10 @@
         <v>38</v>
       </c>
       <c r="N31" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="O31" s="15" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="P31" s="15" t="s">
         <v>404</v>
@@ -3525,13 +3525,13 @@
         <v>25</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D32" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E32" s="12" t="s">
         <v>180</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>181</v>
       </c>
       <c r="F32" s="13">
         <v>45104</v>
@@ -3552,10 +3552,10 @@
         <v>38</v>
       </c>
       <c r="N32" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="O32" s="15" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="P32" s="15" t="s">
         <v>404</v>
@@ -3575,13 +3575,13 @@
         <v>25</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F33" s="13">
         <v>45104</v>
@@ -3602,13 +3602,13 @@
         <v>38</v>
       </c>
       <c r="N33" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="O33" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="P33" s="15" t="s">
         <v>405</v>
-      </c>
-      <c r="O33" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="P33" s="15" t="s">
-        <v>404</v>
       </c>
       <c r="Q33" s="20"/>
       <c r="S33" s="21"/>
@@ -3616,7 +3616,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
         <v>63</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>65</v>
       </c>
       <c r="K34" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
@@ -3654,7 +3654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="19">
         <v>64</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>65</v>
       </c>
       <c r="K35" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
@@ -3692,7 +3692,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="225.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19">
         <v>65</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>24</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>44</v>
@@ -3715,10 +3715,10 @@
         <v>45104.416215277779</v>
       </c>
       <c r="H36" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="I36" s="14" t="s">
         <v>265</v>
-      </c>
-      <c r="I36" s="14" t="s">
-        <v>266</v>
       </c>
       <c r="J36" s="15" t="s">
         <v>38</v>
@@ -3731,13 +3731,13 @@
         <v>38</v>
       </c>
       <c r="N36" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O36" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P36" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q36" s="15"/>
       <c r="R36" s="16"/>
@@ -3746,7 +3746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:20" s="33" customFormat="1" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" s="33" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="23">
         <v>66</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>65</v>
       </c>
       <c r="K37" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L37" s="29"/>
       <c r="M37" s="29"/>
@@ -3784,7 +3784,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19">
         <v>67</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>65</v>
       </c>
       <c r="K38" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
@@ -3822,7 +3822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19">
         <v>68</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>65</v>
       </c>
       <c r="K39" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
@@ -3860,7 +3860,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="19">
         <v>69</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>65</v>
       </c>
       <c r="K40" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
@@ -3898,7 +3898,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19">
         <v>70</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>65</v>
       </c>
       <c r="K41" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
@@ -3936,7 +3936,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="225.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="19">
         <v>71</v>
       </c>
@@ -3959,10 +3959,10 @@
         <v>45104.426342592589</v>
       </c>
       <c r="H42" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="I42" s="14" t="s">
         <v>267</v>
-      </c>
-      <c r="I42" s="14" t="s">
-        <v>268</v>
       </c>
       <c r="J42" s="36" t="s">
         <v>38</v>
@@ -3975,13 +3975,13 @@
         <v>38</v>
       </c>
       <c r="N42" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O42" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P42" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q42" s="15"/>
       <c r="R42" s="16"/>
@@ -3990,7 +3990,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="225.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="19">
         <v>72</v>
       </c>
@@ -4013,10 +4013,10 @@
         <v>45104.427581018521</v>
       </c>
       <c r="H43" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="I43" s="14" t="s">
         <v>269</v>
-      </c>
-      <c r="I43" s="14" t="s">
-        <v>270</v>
       </c>
       <c r="J43" s="15" t="s">
         <v>38</v>
@@ -4029,13 +4029,13 @@
         <v>38</v>
       </c>
       <c r="N43" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O43" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P43" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q43" s="15"/>
       <c r="R43" s="16"/>
@@ -4044,7 +4044,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="225.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="19">
         <v>73</v>
       </c>
@@ -4067,10 +4067,10 @@
         <v>45104.428587962961</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J44" s="15" t="s">
         <v>38</v>
@@ -4083,13 +4083,13 @@
         <v>38</v>
       </c>
       <c r="N44" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O44" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P44" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q44" s="15"/>
       <c r="R44" s="16"/>
@@ -4098,7 +4098,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
         <v>74</v>
       </c>
@@ -4121,10 +4121,10 @@
         <v>45104.429884259262</v>
       </c>
       <c r="H45" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="I45" s="14" t="s">
         <v>272</v>
-      </c>
-      <c r="I45" s="14" t="s">
-        <v>273</v>
       </c>
       <c r="J45" s="15" t="s">
         <v>38</v>
@@ -4137,13 +4137,13 @@
         <v>38</v>
       </c>
       <c r="N45" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O45" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P45" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q45" s="15"/>
       <c r="R45" s="16"/>
@@ -4152,7 +4152,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="19">
         <v>75</v>
       </c>
@@ -4160,13 +4160,13 @@
         <v>25</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D46" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="E46" s="12" t="s">
         <v>341</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>342</v>
       </c>
       <c r="F46" s="13">
         <v>45105</v>
@@ -4175,10 +4175,10 @@
         <v>45105.604085648149</v>
       </c>
       <c r="H46" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="I46" s="14" t="s">
         <v>381</v>
-      </c>
-      <c r="I46" s="14" t="s">
-        <v>382</v>
       </c>
       <c r="J46" s="15" t="s">
         <v>38</v>
@@ -4191,13 +4191,13 @@
         <v>38</v>
       </c>
       <c r="N46" s="15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O46" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P46" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q46" s="15"/>
       <c r="R46" s="16"/>
@@ -4206,7 +4206,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <v>76</v>
       </c>
@@ -4214,13 +4214,13 @@
         <v>25</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D47" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="E47" s="12" t="s">
         <v>343</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>344</v>
       </c>
       <c r="F47" s="13"/>
       <c r="G47" s="14"/>
@@ -4230,7 +4230,7 @@
         <v>65</v>
       </c>
       <c r="K47" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
@@ -4244,7 +4244,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="19">
         <v>77</v>
       </c>
@@ -4252,13 +4252,13 @@
         <v>25</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D48" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="E48" s="12" t="s">
         <v>345</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>346</v>
       </c>
       <c r="F48" s="13"/>
       <c r="G48" s="14"/>
@@ -4268,7 +4268,7 @@
         <v>65</v>
       </c>
       <c r="K48" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
@@ -4282,7 +4282,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="19">
         <v>78</v>
       </c>
@@ -4290,13 +4290,13 @@
         <v>25</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D49" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="E49" s="12" t="s">
         <v>347</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>348</v>
       </c>
       <c r="F49" s="13"/>
       <c r="G49" s="14"/>
@@ -4306,7 +4306,7 @@
         <v>65</v>
       </c>
       <c r="K49" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
@@ -4320,7 +4320,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="19">
         <v>79</v>
       </c>
@@ -4328,13 +4328,13 @@
         <v>25</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D50" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="E50" s="12" t="s">
         <v>349</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>350</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="14"/>
@@ -4344,7 +4344,7 @@
         <v>65</v>
       </c>
       <c r="K50" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
@@ -4358,7 +4358,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="19">
         <v>80</v>
       </c>
@@ -4366,13 +4366,13 @@
         <v>25</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D51" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="E51" s="12" t="s">
         <v>351</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>352</v>
       </c>
       <c r="F51" s="13">
         <v>45105</v>
@@ -4381,10 +4381,10 @@
         <v>45105.675555555557</v>
       </c>
       <c r="H51" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="I51" s="14" t="s">
         <v>384</v>
-      </c>
-      <c r="I51" s="14" t="s">
-        <v>385</v>
       </c>
       <c r="J51" s="15" t="s">
         <v>38</v>
@@ -4397,13 +4397,13 @@
         <v>38</v>
       </c>
       <c r="N51" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="O51" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P51" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q51" s="15"/>
       <c r="R51" s="16"/>
@@ -4412,7 +4412,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="19">
         <v>81</v>
       </c>
@@ -4420,13 +4420,13 @@
         <v>25</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D52" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="E52" s="12" t="s">
         <v>353</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>354</v>
       </c>
       <c r="F52" s="13"/>
       <c r="G52" s="14"/>
@@ -4436,7 +4436,7 @@
         <v>65</v>
       </c>
       <c r="K52" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
@@ -4450,7 +4450,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="19">
         <v>82</v>
       </c>
@@ -4458,13 +4458,13 @@
         <v>25</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D53" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="E53" s="12" t="s">
         <v>355</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>356</v>
       </c>
       <c r="F53" s="13">
         <v>45105</v>
@@ -4473,10 +4473,10 @@
         <v>45105.691793981481</v>
       </c>
       <c r="H53" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="I53" s="14" t="s">
         <v>387</v>
-      </c>
-      <c r="I53" s="14" t="s">
-        <v>388</v>
       </c>
       <c r="J53" s="15" t="s">
         <v>38</v>
@@ -4489,13 +4489,13 @@
         <v>38</v>
       </c>
       <c r="N53" s="15" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="O53" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P53" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q53" s="15"/>
       <c r="R53" s="16"/>
@@ -4504,7 +4504,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="19">
         <v>83</v>
       </c>
@@ -4512,13 +4512,13 @@
         <v>25</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F54" s="13"/>
       <c r="G54" s="14"/>
@@ -4528,7 +4528,7 @@
         <v>65</v>
       </c>
       <c r="K54" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
@@ -4542,7 +4542,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="19">
         <v>84</v>
       </c>
@@ -4550,13 +4550,13 @@
         <v>25</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D55" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="E55" s="12" t="s">
         <v>358</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>359</v>
       </c>
       <c r="F55" s="13">
         <v>45105</v>
@@ -4565,10 +4565,10 @@
         <v>45105.717881944445</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J55" s="15" t="s">
         <v>38</v>
@@ -4581,13 +4581,13 @@
         <v>38</v>
       </c>
       <c r="N55" s="15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="O55" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P55" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q55" s="15"/>
       <c r="R55" s="16"/>
@@ -4596,7 +4596,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="19">
         <v>85</v>
       </c>
@@ -4604,13 +4604,13 @@
         <v>25</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D56" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="E56" s="12" t="s">
         <v>360</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>361</v>
       </c>
       <c r="F56" s="13"/>
       <c r="G56" s="14"/>
@@ -4620,7 +4620,7 @@
         <v>65</v>
       </c>
       <c r="K56" s="15" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
@@ -4634,7 +4634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="19">
         <v>86</v>
       </c>
@@ -4642,13 +4642,13 @@
         <v>25</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D57" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="E57" s="12" t="s">
         <v>362</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>363</v>
       </c>
       <c r="F57" s="13"/>
       <c r="G57" s="14"/>
@@ -4658,7 +4658,7 @@
         <v>65</v>
       </c>
       <c r="K57" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
@@ -4672,7 +4672,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="19">
         <v>87</v>
       </c>
@@ -4680,13 +4680,13 @@
         <v>25</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D58" s="11" t="s">
+        <v>363</v>
+      </c>
+      <c r="E58" s="12" t="s">
         <v>364</v>
-      </c>
-      <c r="E58" s="12" t="s">
-        <v>365</v>
       </c>
       <c r="F58" s="13"/>
       <c r="G58" s="14"/>
@@ -4696,7 +4696,7 @@
         <v>65</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
@@ -4710,7 +4710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="19">
         <v>88</v>
       </c>
@@ -4718,13 +4718,13 @@
         <v>25</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D59" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="E59" s="12" t="s">
         <v>366</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>367</v>
       </c>
       <c r="F59" s="13"/>
       <c r="G59" s="14"/>
@@ -4734,7 +4734,7 @@
         <v>65</v>
       </c>
       <c r="K59" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
@@ -4748,7 +4748,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="19">
         <v>89</v>
       </c>
@@ -4756,13 +4756,13 @@
         <v>25</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D60" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="E60" s="12" t="s">
         <v>368</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>369</v>
       </c>
       <c r="F60" s="13"/>
       <c r="G60" s="14"/>
@@ -4772,7 +4772,7 @@
         <v>65</v>
       </c>
       <c r="K60" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
@@ -4786,7 +4786,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="19">
         <v>90</v>
       </c>
@@ -4794,13 +4794,13 @@
         <v>25</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F61" s="13"/>
       <c r="G61" s="14"/>
@@ -4810,7 +4810,7 @@
         <v>65</v>
       </c>
       <c r="K61" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L61" s="15"/>
       <c r="M61" s="15"/>
@@ -4824,7 +4824,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="19">
         <v>91</v>
       </c>
@@ -4832,13 +4832,13 @@
         <v>25</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F62" s="13"/>
       <c r="G62" s="14"/>
@@ -4848,7 +4848,7 @@
         <v>65</v>
       </c>
       <c r="K62" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L62" s="15"/>
       <c r="M62" s="15"/>
@@ -4862,7 +4862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="19">
         <v>92</v>
       </c>
@@ -4870,13 +4870,13 @@
         <v>25</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D63" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="E63" s="12" t="s">
         <v>374</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>375</v>
       </c>
       <c r="F63" s="13"/>
       <c r="G63" s="14"/>
@@ -4886,7 +4886,7 @@
         <v>65</v>
       </c>
       <c r="K63" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L63" s="15"/>
       <c r="M63" s="15"/>
@@ -4900,7 +4900,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="102.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="19">
         <v>93</v>
       </c>
@@ -4908,13 +4908,13 @@
         <v>25</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D64" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="E64" s="12" t="s">
         <v>376</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>377</v>
       </c>
       <c r="F64" s="13"/>
       <c r="G64" s="14"/>
@@ -4924,7 +4924,7 @@
         <v>65</v>
       </c>
       <c r="K64" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L64" s="15"/>
       <c r="M64" s="15"/>
@@ -4938,7 +4938,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="19">
         <v>122</v>
       </c>
@@ -4946,13 +4946,13 @@
         <v>25</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D65" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E65" s="12" t="s">
         <v>99</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>100</v>
       </c>
       <c r="F65" s="13"/>
       <c r="G65" s="14"/>
@@ -4962,7 +4962,7 @@
         <v>65</v>
       </c>
       <c r="K65" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L65" s="15"/>
       <c r="M65" s="15"/>
@@ -4976,7 +4976,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="19">
         <v>123</v>
       </c>
@@ -4984,13 +4984,13 @@
         <v>25</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D66" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E66" s="12" t="s">
         <v>101</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>102</v>
       </c>
       <c r="F66" s="13"/>
       <c r="G66" s="14"/>
@@ -5000,7 +5000,7 @@
         <v>65</v>
       </c>
       <c r="K66" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L66" s="15"/>
       <c r="M66" s="15"/>
@@ -5014,7 +5014,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="19">
         <v>124</v>
       </c>
@@ -5022,13 +5022,13 @@
         <v>25</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D67" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E67" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="E67" s="12" t="s">
-        <v>104</v>
       </c>
       <c r="F67" s="13">
         <v>45104</v>
@@ -5037,11 +5037,11 @@
         <v>45104.434178240743</v>
       </c>
       <c r="H67" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="I67" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="I67" s="14" t="s">
-        <v>275</v>
-      </c>
       <c r="J67" s="15" t="s">
         <v>38</v>
       </c>
@@ -5052,13 +5052,13 @@
         <v>38</v>
       </c>
       <c r="N67" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O67" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P67" s="15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="Q67" s="15"/>
       <c r="R67" s="16"/>
@@ -5067,7 +5067,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="19">
         <v>125</v>
       </c>
@@ -5075,13 +5075,13 @@
         <v>25</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D68" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E68" s="12" t="s">
         <v>105</v>
-      </c>
-      <c r="E68" s="12" t="s">
-        <v>106</v>
       </c>
       <c r="F68" s="13"/>
       <c r="G68" s="14"/>
@@ -5091,7 +5091,7 @@
         <v>65</v>
       </c>
       <c r="K68" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L68" s="15"/>
       <c r="M68" s="15"/>
@@ -5105,7 +5105,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="19">
         <v>126</v>
       </c>
@@ -5113,13 +5113,13 @@
         <v>25</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D69" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E69" s="12" t="s">
         <v>107</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>108</v>
       </c>
       <c r="F69" s="13"/>
       <c r="G69" s="14"/>
@@ -5129,7 +5129,7 @@
         <v>65</v>
       </c>
       <c r="K69" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L69" s="15"/>
       <c r="M69" s="15"/>
@@ -5143,7 +5143,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="19">
         <v>127</v>
       </c>
@@ -5151,13 +5151,13 @@
         <v>25</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D70" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E70" s="12" t="s">
         <v>109</v>
-      </c>
-      <c r="E70" s="12" t="s">
-        <v>110</v>
       </c>
       <c r="F70" s="13"/>
       <c r="G70" s="14"/>
@@ -5167,7 +5167,7 @@
         <v>65</v>
       </c>
       <c r="K70" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L70" s="15"/>
       <c r="M70" s="15"/>
@@ -5181,7 +5181,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="19">
         <v>128</v>
       </c>
@@ -5189,13 +5189,13 @@
         <v>25</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D71" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E71" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="E71" s="12" t="s">
-        <v>112</v>
       </c>
       <c r="F71" s="13"/>
       <c r="G71" s="14"/>
@@ -5205,7 +5205,7 @@
         <v>65</v>
       </c>
       <c r="K71" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L71" s="15"/>
       <c r="M71" s="15"/>
@@ -5219,7 +5219,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="19">
         <v>129</v>
       </c>
@@ -5227,13 +5227,13 @@
         <v>25</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F72" s="13">
         <v>45104</v>
@@ -5242,10 +5242,10 @@
         <v>45104.435486111113</v>
       </c>
       <c r="H72" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="I72" s="14" t="s">
         <v>276</v>
-      </c>
-      <c r="I72" s="14" t="s">
-        <v>277</v>
       </c>
       <c r="J72" s="15" t="s">
         <v>38</v>
@@ -5258,13 +5258,13 @@
         <v>38</v>
       </c>
       <c r="N72" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O72" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P72" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q72" s="15"/>
       <c r="R72" s="16"/>
@@ -5273,7 +5273,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="19">
         <v>130</v>
       </c>
@@ -5281,13 +5281,13 @@
         <v>25</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D73" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E73" s="12" t="s">
         <v>115</v>
-      </c>
-      <c r="E73" s="12" t="s">
-        <v>116</v>
       </c>
       <c r="F73" s="13">
         <v>45104</v>
@@ -5296,10 +5296,10 @@
         <v>45104.436909722222</v>
       </c>
       <c r="H73" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="I73" s="14" t="s">
         <v>278</v>
-      </c>
-      <c r="I73" s="14" t="s">
-        <v>279</v>
       </c>
       <c r="J73" s="15" t="s">
         <v>38</v>
@@ -5312,13 +5312,13 @@
         <v>38</v>
       </c>
       <c r="N73" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O73" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P73" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q73" s="15"/>
       <c r="R73" s="16"/>
@@ -5327,7 +5327,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="19">
         <v>131</v>
       </c>
@@ -5335,13 +5335,13 @@
         <v>25</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D74" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E74" s="12" t="s">
         <v>117</v>
-      </c>
-      <c r="E74" s="12" t="s">
-        <v>118</v>
       </c>
       <c r="F74" s="13">
         <v>45104</v>
@@ -5350,10 +5350,10 @@
         <v>45104.438668981478</v>
       </c>
       <c r="H74" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I74" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J74" s="15" t="s">
         <v>38</v>
@@ -5366,13 +5366,13 @@
         <v>38</v>
       </c>
       <c r="N74" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O74" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P74" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q74" s="15"/>
       <c r="R74" s="16"/>
@@ -5381,7 +5381,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="19">
         <v>132</v>
       </c>
@@ -5389,13 +5389,13 @@
         <v>25</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F75" s="13">
         <v>45104</v>
@@ -5404,10 +5404,10 @@
         <v>45104.439479166664</v>
       </c>
       <c r="H75" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="I75" s="14" t="s">
         <v>281</v>
-      </c>
-      <c r="I75" s="14" t="s">
-        <v>282</v>
       </c>
       <c r="J75" s="15" t="s">
         <v>38</v>
@@ -5420,13 +5420,13 @@
         <v>38</v>
       </c>
       <c r="N75" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O75" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P75" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q75" s="15"/>
       <c r="R75" s="16"/>
@@ -5435,7 +5435,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="19">
         <v>133</v>
       </c>
@@ -5443,13 +5443,13 @@
         <v>25</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F76" s="13"/>
       <c r="G76" s="14"/>
@@ -5459,7 +5459,7 @@
         <v>65</v>
       </c>
       <c r="K76" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L76" s="15"/>
       <c r="M76" s="15"/>
@@ -5473,7 +5473,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="19">
         <v>134</v>
       </c>
@@ -5481,13 +5481,13 @@
         <v>25</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F77" s="13"/>
       <c r="G77" s="14"/>
@@ -5497,7 +5497,7 @@
         <v>65</v>
       </c>
       <c r="K77" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L77" s="15"/>
       <c r="M77" s="15"/>
@@ -5511,7 +5511,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="19">
         <v>135</v>
       </c>
@@ -5519,13 +5519,13 @@
         <v>25</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F78" s="13">
         <v>45104</v>
@@ -5534,10 +5534,10 @@
         <v>45104.442962962959</v>
       </c>
       <c r="H78" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="I78" s="14" t="s">
         <v>283</v>
-      </c>
-      <c r="I78" s="14" t="s">
-        <v>284</v>
       </c>
       <c r="J78" s="15" t="s">
         <v>38</v>
@@ -5550,13 +5550,13 @@
         <v>38</v>
       </c>
       <c r="N78" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O78" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P78" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q78" s="15"/>
       <c r="R78" s="16"/>
@@ -5565,7 +5565,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="19">
         <v>136</v>
       </c>
@@ -5573,13 +5573,13 @@
         <v>25</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E79" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F79" s="13"/>
       <c r="G79" s="14"/>
@@ -5589,7 +5589,7 @@
         <v>65</v>
       </c>
       <c r="K79" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M79" s="15"/>
       <c r="N79" s="15"/>
@@ -5602,7 +5602,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="19">
         <v>137</v>
       </c>
@@ -5610,13 +5610,13 @@
         <v>25</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E80" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F80" s="13">
         <v>45104</v>
@@ -5625,10 +5625,10 @@
         <v>45104.443761574075</v>
       </c>
       <c r="H80" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="I80" s="14" t="s">
         <v>285</v>
-      </c>
-      <c r="I80" s="14" t="s">
-        <v>286</v>
       </c>
       <c r="J80" s="15" t="s">
         <v>38</v>
@@ -5641,13 +5641,13 @@
         <v>38</v>
       </c>
       <c r="N80" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O80" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P80" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q80" s="15"/>
       <c r="R80" s="16"/>
@@ -5656,7 +5656,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="19">
         <v>138</v>
       </c>
@@ -5664,13 +5664,13 @@
         <v>25</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F81" s="13">
         <v>45104</v>
@@ -5679,10 +5679,10 @@
         <v>45104.444768518515</v>
       </c>
       <c r="H81" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="I81" s="14" t="s">
         <v>287</v>
-      </c>
-      <c r="I81" s="14" t="s">
-        <v>288</v>
       </c>
       <c r="J81" s="15" t="s">
         <v>38</v>
@@ -5695,13 +5695,13 @@
         <v>38</v>
       </c>
       <c r="N81" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O81" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P81" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q81" s="15"/>
       <c r="R81" s="16"/>
@@ -5710,7 +5710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="19">
         <v>139</v>
       </c>
@@ -5718,13 +5718,13 @@
         <v>25</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F82" s="13"/>
       <c r="G82" s="14"/>
@@ -5734,7 +5734,7 @@
         <v>65</v>
       </c>
       <c r="K82" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L82" s="15"/>
       <c r="M82" s="15"/>
@@ -5748,7 +5748,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="19">
         <v>140</v>
       </c>
@@ -5756,13 +5756,13 @@
         <v>25</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E83" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F83" s="13"/>
       <c r="G83" s="14"/>
@@ -5772,7 +5772,7 @@
         <v>65</v>
       </c>
       <c r="K83" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L83" s="15"/>
       <c r="M83" s="15"/>
@@ -5786,7 +5786,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="19">
         <v>141</v>
       </c>
@@ -5794,13 +5794,13 @@
         <v>25</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E84" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F84" s="13">
         <v>45104</v>
@@ -5809,10 +5809,10 @@
         <v>45104.445601851854</v>
       </c>
       <c r="H84" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="I84" s="38" t="s">
         <v>289</v>
-      </c>
-      <c r="I84" s="38" t="s">
-        <v>290</v>
       </c>
       <c r="J84" s="15" t="s">
         <v>38</v>
@@ -5825,13 +5825,13 @@
         <v>38</v>
       </c>
       <c r="N84" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O84" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P84" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q84" s="15"/>
       <c r="R84" s="16"/>
@@ -5840,7 +5840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="19">
         <v>142</v>
       </c>
@@ -5848,13 +5848,13 @@
         <v>25</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F85" s="13">
         <v>45104</v>
@@ -5863,10 +5863,10 @@
         <v>45104.446585648147</v>
       </c>
       <c r="H85" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="I85" s="14" t="s">
         <v>291</v>
-      </c>
-      <c r="I85" s="14" t="s">
-        <v>292</v>
       </c>
       <c r="J85" s="15" t="s">
         <v>38</v>
@@ -5879,13 +5879,13 @@
         <v>38</v>
       </c>
       <c r="N85" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O85" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P85" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q85" s="15"/>
       <c r="R85" s="16"/>
@@ -5894,7 +5894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="19">
         <v>143</v>
       </c>
@@ -5902,13 +5902,13 @@
         <v>25</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E86" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F86" s="13">
         <v>45104</v>
@@ -5917,10 +5917,10 @@
         <v>45104.447384259256</v>
       </c>
       <c r="H86" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="I86" s="14" t="s">
         <v>293</v>
-      </c>
-      <c r="I86" s="14" t="s">
-        <v>294</v>
       </c>
       <c r="J86" s="15" t="s">
         <v>38</v>
@@ -5933,13 +5933,13 @@
         <v>38</v>
       </c>
       <c r="N86" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O86" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P86" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q86" s="15"/>
       <c r="R86" s="16"/>
@@ -5948,7 +5948,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="19">
         <v>144</v>
       </c>
@@ -5956,13 +5956,13 @@
         <v>25</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E87" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F87" s="13">
         <v>45104</v>
@@ -5971,10 +5971,10 @@
         <v>45104.449189814812</v>
       </c>
       <c r="H87" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="I87" s="14" t="s">
         <v>295</v>
-      </c>
-      <c r="I87" s="14" t="s">
-        <v>296</v>
       </c>
       <c r="J87" s="15" t="s">
         <v>38</v>
@@ -5987,13 +5987,13 @@
         <v>38</v>
       </c>
       <c r="N87" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O87" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P87" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q87" s="15"/>
       <c r="R87" s="16"/>
@@ -6002,7 +6002,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="19">
         <v>145</v>
       </c>
@@ -6010,13 +6010,13 @@
         <v>25</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E88" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F88" s="13"/>
       <c r="G88" s="14"/>
@@ -6026,7 +6026,7 @@
         <v>65</v>
       </c>
       <c r="K88" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L88" s="15"/>
       <c r="M88" s="15"/>
@@ -6040,7 +6040,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="98.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" ht="98.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="19">
         <v>146</v>
       </c>
@@ -6048,13 +6048,13 @@
         <v>25</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E89" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F89" s="13">
         <v>45104</v>
@@ -6063,10 +6063,10 @@
         <v>45104.450011574074</v>
       </c>
       <c r="H89" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="I89" s="14" t="s">
         <v>297</v>
-      </c>
-      <c r="I89" s="14" t="s">
-        <v>298</v>
       </c>
       <c r="J89" s="15" t="s">
         <v>38</v>
@@ -6079,13 +6079,13 @@
         <v>38</v>
       </c>
       <c r="N89" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O89" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P89" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q89" s="15"/>
       <c r="R89" s="16"/>
@@ -6094,7 +6094,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="19">
         <v>147</v>
       </c>
@@ -6102,13 +6102,13 @@
         <v>25</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D90" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="E90" s="12" t="s">
         <v>184</v>
-      </c>
-      <c r="E90" s="12" t="s">
-        <v>185</v>
       </c>
       <c r="F90" s="13">
         <v>45104</v>
@@ -6117,10 +6117,10 @@
         <v>45104.450856481482</v>
       </c>
       <c r="H90" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="I90" s="14" t="s">
         <v>299</v>
-      </c>
-      <c r="I90" s="14" t="s">
-        <v>300</v>
       </c>
       <c r="J90" s="15" t="s">
         <v>38</v>
@@ -6142,7 +6142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="19">
         <v>148</v>
       </c>
@@ -6150,13 +6150,13 @@
         <v>25</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E91" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F91" s="13"/>
       <c r="G91" s="14"/>
@@ -6166,7 +6166,7 @@
         <v>65</v>
       </c>
       <c r="K91" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L91" s="15"/>
       <c r="M91" s="15"/>
@@ -6180,7 +6180,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="19">
         <v>149</v>
       </c>
@@ -6188,13 +6188,13 @@
         <v>25</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E92" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F92" s="13"/>
       <c r="G92" s="14"/>
@@ -6204,7 +6204,7 @@
         <v>65</v>
       </c>
       <c r="K92" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L92" s="15"/>
       <c r="M92" s="15"/>
@@ -6218,7 +6218,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="19">
         <v>150</v>
       </c>
@@ -6226,13 +6226,13 @@
         <v>25</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E93" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F93" s="13"/>
       <c r="G93" s="14"/>
@@ -6242,7 +6242,7 @@
         <v>65</v>
       </c>
       <c r="K93" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L93" s="15"/>
       <c r="M93" s="15"/>
@@ -6256,7 +6256,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="19">
         <v>151</v>
       </c>
@@ -6264,13 +6264,13 @@
         <v>25</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E94" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F94" s="13">
         <v>45104</v>
@@ -6279,10 +6279,10 @@
         <v>45104.451840277776</v>
       </c>
       <c r="H94" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="I94" s="14" t="s">
         <v>301</v>
-      </c>
-      <c r="I94" s="14" t="s">
-        <v>302</v>
       </c>
       <c r="J94" s="15" t="s">
         <v>38</v>
@@ -6295,13 +6295,13 @@
         <v>38</v>
       </c>
       <c r="N94" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O94" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P94" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q94" s="15"/>
       <c r="R94" s="16"/>
@@ -6310,7 +6310,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="19">
         <v>152</v>
       </c>
@@ -6318,13 +6318,13 @@
         <v>25</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F95" s="13"/>
       <c r="G95" s="14"/>
@@ -6334,7 +6334,7 @@
         <v>65</v>
       </c>
       <c r="K95" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L95" s="15"/>
       <c r="M95" s="15"/>
@@ -6348,7 +6348,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="19">
         <v>153</v>
       </c>
@@ -6356,13 +6356,13 @@
         <v>25</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F96" s="13">
         <v>45111</v>
@@ -6371,10 +6371,10 @@
         <v>45111.63380787037</v>
       </c>
       <c r="H96" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I96" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J96" s="15" t="s">
         <v>38</v>
@@ -6387,13 +6387,13 @@
         <v>38</v>
       </c>
       <c r="N96" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O96" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P96" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q96" s="15"/>
       <c r="R96" s="16"/>
@@ -6402,7 +6402,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="19">
         <v>154</v>
       </c>
@@ -6410,13 +6410,13 @@
         <v>25</v>
       </c>
       <c r="C97" s="42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F97" s="13"/>
       <c r="G97" s="14"/>
@@ -6426,7 +6426,7 @@
         <v>65</v>
       </c>
       <c r="K97" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L97" s="15"/>
       <c r="M97" s="15"/>
@@ -6440,7 +6440,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="19">
         <v>155</v>
       </c>
@@ -6448,13 +6448,13 @@
         <v>25</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F98" s="13"/>
       <c r="G98" s="14"/>
@@ -6464,7 +6464,7 @@
         <v>65</v>
       </c>
       <c r="K98" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L98" s="15"/>
       <c r="M98" s="15"/>
@@ -6478,7 +6478,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="19">
         <v>156</v>
       </c>
@@ -6486,13 +6486,13 @@
         <v>25</v>
       </c>
       <c r="C99" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D99" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E99" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F99" s="13"/>
       <c r="G99" s="14"/>
@@ -6502,7 +6502,7 @@
         <v>65</v>
       </c>
       <c r="K99" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L99" s="15"/>
       <c r="M99" s="15"/>
@@ -6516,7 +6516,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="19">
         <v>157</v>
       </c>
@@ -6524,13 +6524,13 @@
         <v>25</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E100" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F100" s="13"/>
       <c r="G100" s="14"/>
@@ -6540,7 +6540,7 @@
         <v>65</v>
       </c>
       <c r="K100" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L100" s="15"/>
       <c r="M100" s="15"/>
@@ -6554,7 +6554,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="19">
         <v>158</v>
       </c>
@@ -6562,13 +6562,13 @@
         <v>25</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E101" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F101" s="13">
         <v>45104</v>
@@ -6577,10 +6577,10 @@
         <v>45104.454525462963</v>
       </c>
       <c r="H101" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="I101" s="14" t="s">
         <v>303</v>
-      </c>
-      <c r="I101" s="14" t="s">
-        <v>304</v>
       </c>
       <c r="J101" s="15" t="s">
         <v>38</v>
@@ -6593,13 +6593,13 @@
         <v>38</v>
       </c>
       <c r="N101" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O101" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P101" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q101" s="15"/>
       <c r="R101" s="16"/>
@@ -6608,7 +6608,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="19">
         <v>159</v>
       </c>
@@ -6616,13 +6616,13 @@
         <v>25</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E102" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F102" s="13">
         <v>45104</v>
@@ -6631,10 +6631,10 @@
         <v>45104.455439814818</v>
       </c>
       <c r="H102" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="I102" s="14" t="s">
         <v>305</v>
-      </c>
-      <c r="I102" s="14" t="s">
-        <v>306</v>
       </c>
       <c r="J102" s="15" t="s">
         <v>38</v>
@@ -6647,13 +6647,13 @@
         <v>38</v>
       </c>
       <c r="N102" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O102" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P102" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q102" s="15"/>
       <c r="R102" s="16"/>
@@ -6662,7 +6662,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="19">
         <v>160</v>
       </c>
@@ -6670,13 +6670,13 @@
         <v>25</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F103" s="13">
         <v>45104</v>
@@ -6685,10 +6685,10 @@
         <v>45104.456284722219</v>
       </c>
       <c r="H103" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="I103" s="14" t="s">
         <v>307</v>
-      </c>
-      <c r="I103" s="14" t="s">
-        <v>308</v>
       </c>
       <c r="J103" s="15" t="s">
         <v>38</v>
@@ -6701,13 +6701,13 @@
         <v>38</v>
       </c>
       <c r="N103" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O103" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P103" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q103" s="15"/>
       <c r="R103" s="16"/>
@@ -6716,7 +6716,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="19">
         <v>161</v>
       </c>
@@ -6724,13 +6724,13 @@
         <v>25</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F104" s="13">
         <v>45104</v>
@@ -6739,10 +6739,10 @@
         <v>45104.457465277781</v>
       </c>
       <c r="H104" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="I104" s="14" t="s">
         <v>309</v>
-      </c>
-      <c r="I104" s="14" t="s">
-        <v>310</v>
       </c>
       <c r="J104" s="15" t="s">
         <v>38</v>
@@ -6755,13 +6755,13 @@
         <v>38</v>
       </c>
       <c r="N104" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O104" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P104" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q104" s="15"/>
       <c r="R104" s="16"/>
@@ -6770,7 +6770,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:20" s="33" customFormat="1" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:20" s="33" customFormat="1" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="23">
         <v>162</v>
       </c>
@@ -6778,13 +6778,13 @@
         <v>25</v>
       </c>
       <c r="C105" s="24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D105" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E105" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F105" s="26">
         <v>45104</v>
@@ -6793,10 +6793,10 @@
         <v>45104.772928240738</v>
       </c>
       <c r="H105" s="27" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I105" s="27" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J105" s="29" t="s">
         <v>38</v>
@@ -6809,13 +6809,13 @@
         <v>38</v>
       </c>
       <c r="N105" s="29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O105" s="29" t="s">
         <v>38</v>
       </c>
       <c r="P105" s="29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q105" s="29"/>
       <c r="R105" s="30"/>
@@ -6824,7 +6824,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="19">
         <v>163</v>
       </c>
@@ -6832,13 +6832,13 @@
         <v>25</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D106" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E106" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F106" s="13"/>
       <c r="G106" s="14"/>
@@ -6848,7 +6848,7 @@
         <v>65</v>
       </c>
       <c r="K106" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L106" s="15"/>
       <c r="M106" s="15"/>
@@ -6862,7 +6862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="19">
         <v>164</v>
       </c>
@@ -6870,13 +6870,13 @@
         <v>25</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D107" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F107" s="13">
         <v>45104</v>
@@ -6885,10 +6885,10 @@
         <v>45104.464988425927</v>
       </c>
       <c r="H107" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="I107" s="14" t="s">
         <v>311</v>
-      </c>
-      <c r="I107" s="14" t="s">
-        <v>312</v>
       </c>
       <c r="J107" s="15" t="s">
         <v>38</v>
@@ -6901,13 +6901,13 @@
         <v>38</v>
       </c>
       <c r="N107" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O107" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P107" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q107" s="15"/>
       <c r="R107" s="16"/>
@@ -6916,7 +6916,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="98.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:20" ht="98.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="19">
         <v>165</v>
       </c>
@@ -6924,13 +6924,13 @@
         <v>25</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E108" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F108" s="13">
         <v>45104</v>
@@ -6939,10 +6939,10 @@
         <v>45104.773680555554</v>
       </c>
       <c r="H108" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="I108" s="14" t="s">
         <v>313</v>
-      </c>
-      <c r="I108" s="14" t="s">
-        <v>314</v>
       </c>
       <c r="J108" s="15" t="s">
         <v>38</v>
@@ -6955,13 +6955,13 @@
         <v>38</v>
       </c>
       <c r="N108" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O108" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P108" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q108" s="15"/>
       <c r="R108" s="16"/>
@@ -6970,7 +6970,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="19">
         <v>166</v>
       </c>
@@ -6978,13 +6978,13 @@
         <v>25</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E109" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F109" s="13">
         <v>45104</v>
@@ -6993,10 +6993,10 @@
         <v>45104.774641203701</v>
       </c>
       <c r="H109" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="I109" s="14" t="s">
         <v>315</v>
-      </c>
-      <c r="I109" s="14" t="s">
-        <v>316</v>
       </c>
       <c r="J109" s="15" t="s">
         <v>38</v>
@@ -7009,13 +7009,13 @@
         <v>38</v>
       </c>
       <c r="N109" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O109" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P109" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q109" s="15"/>
       <c r="R109" s="16"/>
@@ -7024,7 +7024,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="19">
         <v>167</v>
       </c>
@@ -7032,13 +7032,13 @@
         <v>25</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E110" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F110" s="13">
         <v>45104</v>
@@ -7047,10 +7047,10 @@
         <v>45104.775740740741</v>
       </c>
       <c r="H110" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="I110" s="14" t="s">
         <v>317</v>
-      </c>
-      <c r="I110" s="14" t="s">
-        <v>318</v>
       </c>
       <c r="J110" s="15" t="s">
         <v>38</v>
@@ -7063,13 +7063,13 @@
         <v>38</v>
       </c>
       <c r="N110" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O110" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P110" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q110" s="15"/>
       <c r="R110" s="16"/>
@@ -7078,7 +7078,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="19">
         <v>168</v>
       </c>
@@ -7086,13 +7086,13 @@
         <v>25</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E111" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F111" s="13"/>
       <c r="G111" s="14"/>
@@ -7102,7 +7102,7 @@
         <v>65</v>
       </c>
       <c r="K111" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L111" s="15"/>
       <c r="M111" s="15"/>
@@ -7116,7 +7116,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="19">
         <v>169</v>
       </c>
@@ -7124,13 +7124,13 @@
         <v>25</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D112" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E112" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F112" s="13">
         <v>45104</v>
@@ -7139,10 +7139,10 @@
         <v>45104.776620370372</v>
       </c>
       <c r="H112" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="I112" s="14" t="s">
         <v>319</v>
-      </c>
-      <c r="I112" s="14" t="s">
-        <v>320</v>
       </c>
       <c r="J112" s="15" t="s">
         <v>38</v>
@@ -7155,13 +7155,13 @@
         <v>38</v>
       </c>
       <c r="N112" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O112" s="15" t="s">
         <v>38</v>
       </c>
       <c r="P112" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q112" s="15"/>
       <c r="R112" s="16"/>
@@ -7170,7 +7170,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="1:21" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:21" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="19">
         <v>369</v>
       </c>
@@ -7181,7 +7181,7 @@
         <v>24</v>
       </c>
       <c r="D113" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E113" s="12"/>
       <c r="F113" s="13">
@@ -7191,10 +7191,10 @@
         <v>45104.777511574073</v>
       </c>
       <c r="H113" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="I113" s="14" t="s">
         <v>321</v>
-      </c>
-      <c r="I113" s="14" t="s">
-        <v>322</v>
       </c>
       <c r="J113" s="15" t="s">
         <v>38</v>
@@ -7216,7 +7216,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="114" spans="1:21" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:21" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="19">
         <v>370</v>
       </c>
@@ -7224,10 +7224,10 @@
         <v>25</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D114" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E114" s="12"/>
       <c r="F114" s="13">
@@ -7237,10 +7237,10 @@
         <v>45105.704733796294</v>
       </c>
       <c r="H114" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="I114" s="14" t="s">
         <v>398</v>
-      </c>
-      <c r="I114" s="14" t="s">
-        <v>399</v>
       </c>
       <c r="J114" s="15" t="s">
         <v>38</v>
@@ -7253,7 +7253,7 @@
         <v>38</v>
       </c>
       <c r="P114" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q114" s="15"/>
       <c r="R114" s="16"/>
@@ -7262,7 +7262,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="115" spans="1:21" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:21" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="19">
         <v>373</v>
       </c>
@@ -7270,10 +7270,10 @@
         <v>25</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D115" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E115" s="12"/>
       <c r="F115" s="13">
@@ -7283,10 +7283,10 @@
         <v>45104.778263888889</v>
       </c>
       <c r="H115" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I115" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J115" s="15" t="s">
         <v>38</v>
@@ -7308,7 +7308,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="116" spans="1:21" ht="100.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:21" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="19">
         <v>374</v>
       </c>
@@ -7316,10 +7316,10 @@
         <v>25</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D116" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E116" s="12"/>
       <c r="F116" s="13">
@@ -7329,10 +7329,10 @@
         <v>45104.779027777775</v>
       </c>
       <c r="H116" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="I116" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="I116" s="14" t="s">
-        <v>326</v>
       </c>
       <c r="J116" s="15" t="s">
         <v>38</v>
@@ -16954,16 +16954,7 @@
       <c r="T736" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T116" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="VALIDAZIONE_LDO_TIMEOUT"/>
-        <filter val="VALIDAZIONE_RAD_TIMEOUT"/>
-        <filter val="VALIDAZIONE_RSA_TIMEOUT"/>
-        <filter val="VALIDAZIONE_VPS_TIMEOUT"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A9:T116" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>

</xml_diff>